<commit_message>
Completed translation of G★4 quest information.
</commit_message>
<xml_diff>
--- a/data_G.xlsx
+++ b/data_G.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19007"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2196" uniqueCount="840">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2282" uniqueCount="893">
   <si>
     <t>questName</t>
   </si>
@@ -1762,16 +1762,13 @@
     <t>絆の証？雪山の獰猛大決戦</t>
   </si>
   <si>
+    <t>인연의 증거? 설산의 영맹대결전</t>
+  </si>
+  <si>
     <t>G★4</t>
   </si>
   <si>
-    <t>雪山</t>
-  </si>
-  <si>
-    <t>全ての大型モンスターの狩猟</t>
-  </si>
-  <si>
-    <t>龍歴院ポイント２５００pts入手</t>
+    <t>용역원(龍歴院)포인트２５００pts입수</t>
   </si>
   <si>
     <t>4400z</t>
@@ -1783,10 +1780,10 @@
     <t>金と銀がもたらす悲哀</t>
   </si>
   <si>
-    <t>遺群嶺</t>
-  </si>
-  <si>
-    <t>リオレウス希少種１頭とリオレイア希少種１頭の狩猟</t>
+    <t>금과 은이 가져오는 비애</t>
+  </si>
+  <si>
+    <t>리오레우스 희소종(リオレウス希少種) 1마리와 리오레이아 희소종(リオレイア希少種) 1마리 수렵</t>
   </si>
   <si>
     <t>5800z</t>
@@ -1798,13 +1795,13 @@
     <t>感動の生まれる瞬間</t>
   </si>
   <si>
-    <t>闘技場</t>
-  </si>
-  <si>
-    <t>イビルジョー１頭とラージャン１頭の狩猟</t>
-  </si>
-  <si>
-    <t>乗りによるダウンを２回成功</t>
+    <t>감동적인 탄생의 순간</t>
+  </si>
+  <si>
+    <t>이빌죠(イビルジョー) 1마리와 라쟌(ラージャン) 1마리 수렵</t>
+  </si>
+  <si>
+    <t>단차에 의한 다운을２회 성공</t>
   </si>
   <si>
     <t>3800z</t>
@@ -1819,25 +1816,19 @@
     <t>先生の弱点は獰猛な重甲虫</t>
   </si>
   <si>
-    <t>原生林</t>
-  </si>
-  <si>
-    <t>ゲネル・セルタス１匹の狩猟</t>
-  </si>
-  <si>
-    <t>ゲネル・セルタスの頭部と尻尾破壊</t>
+    <t>선생의 약점은 영맹한 중갑충</t>
+  </si>
+  <si>
+    <t>게넬・셀타스(ゲネル・セルタス)의 머리와 꼬리 파괴</t>
   </si>
   <si>
     <t>採掘場を取り戻せ！</t>
   </si>
   <si>
-    <t>地底火山</t>
-  </si>
-  <si>
-    <t>ウラガンキン１頭の狩猟</t>
-  </si>
-  <si>
-    <t>ウラガンキンの顎と背中破壊</t>
+    <t>채굴장을 되찾아라!</t>
+  </si>
+  <si>
+    <t>우라간킨(ウラガンキン)의 턱과 등 파괴</t>
   </si>
   <si>
     <t>21000z</t>
@@ -1846,7 +1837,7 @@
     <t>鎧・砕・斬の包囲網を越えて</t>
   </si>
   <si>
-    <t>火山</t>
+    <t>개・쇄・참의 포위망을 넘어서</t>
   </si>
   <si>
     <t>4600z</t>
@@ -1858,13 +1849,13 @@
     <t>金色超巨星</t>
   </si>
   <si>
-    <t>密林</t>
-  </si>
-  <si>
-    <t>ラージャン１頭の狩猟</t>
-  </si>
-  <si>
-    <t>ラージャンの角破壊</t>
+    <t>금빛초거성</t>
+  </si>
+  <si>
+    <t>라쟌(ラージャン) 1마리 수렵</t>
+  </si>
+  <si>
+    <t>라쟌(ラージャン)의 뿔 파괴</t>
   </si>
   <si>
     <t>32400z</t>
@@ -1873,10 +1864,13 @@
     <t>終末の時</t>
   </si>
   <si>
-    <t>溶岩島</t>
-  </si>
-  <si>
-    <t>ミラボレアスの討伐または撃退</t>
+    <t>종말의 때</t>
+  </si>
+  <si>
+    <t>용암도(溶岩島)</t>
+  </si>
+  <si>
+    <t>밀라보레아스(ミラボレアス) 토벌 혹은 격퇴</t>
   </si>
   <si>
     <t>45000z</t>
@@ -1885,22 +1879,25 @@
     <t>獰猛な砕竜は、孤島で何を思う</t>
   </si>
   <si>
-    <t>孤島</t>
-  </si>
-  <si>
-    <t>ブラキディオス１頭の狩猟</t>
-  </si>
-  <si>
-    <t>ブラキディオスの頭部破壊と尻尾切断</t>
+    <t>영맹한 쇄룡은, 고도에서 무엇을 생각하나</t>
+  </si>
+  <si>
+    <t>브라키디오스(ブラキディオス) 1마리 수렵</t>
+  </si>
+  <si>
+    <t>브라키디오스(ブラキディオス)의 머리 파괴와 꼬리 절단</t>
   </si>
   <si>
     <t>大地に踊る黄金</t>
   </si>
   <si>
-    <t>リオレイア希少種１頭の狩猟</t>
-  </si>
-  <si>
-    <t>リオレイア希少種の翼と背中破壊</t>
+    <t>대지에서 춤추는 황금</t>
+  </si>
+  <si>
+    <t>리오레이아 희소종(リオレイア希少種) 1마리 수렵</t>
+  </si>
+  <si>
+    <t>리오레이아 희소종(リオレイア希少種)의 날개와 등 파괴</t>
   </si>
   <si>
     <t>3500z</t>
@@ -1912,7 +1909,7 @@
     <t>狩魂よ砂中に眠れ</t>
   </si>
   <si>
-    <t>砂漠</t>
+    <t>사냥꾼의 혼이여 모래속에 잠들어라</t>
   </si>
   <si>
     <t>4700z</t>
@@ -1924,43 +1921,46 @@
     <t>虚空に消え去りし者</t>
   </si>
   <si>
-    <t>森丘</t>
-  </si>
-  <si>
-    <t>オオナズチの討伐または撃退</t>
-  </si>
-  <si>
-    <t>オオナズチの角破壊と尻尾切断</t>
+    <t>허공에 사라져 없어진 자</t>
+  </si>
+  <si>
+    <t>오나즈치(オオナズチ) 토벌 혹은 격퇴</t>
+  </si>
+  <si>
+    <t>오나즈치(オオナズチ)의 뿔 파괴와 꼬리 절단</t>
   </si>
   <si>
     <t>雪に紛れしドスギアノス</t>
   </si>
   <si>
-    <t>氷海</t>
-  </si>
-  <si>
-    <t>ドスギアノス２頭の狩猟</t>
+    <t>눈속에 헤매이는 도스 기아노스</t>
+  </si>
+  <si>
+    <t>도스기아노스(ドスギアノス) 2마리 수렵</t>
   </si>
   <si>
     <t>天を廻りて、冥界に堕つ</t>
   </si>
   <si>
-    <t>ゴア・マガラ１頭の狩猟</t>
-  </si>
-  <si>
-    <t>ゴア・マガラの右翼脚破壊</t>
+    <t>하늘을 돌아, 명계에 내리다</t>
+  </si>
+  <si>
+    <t>고어・마가라(ゴア・マガラ)의 우측 날개 다리 파괴</t>
   </si>
   <si>
     <t>極天より来たる、崩せし神</t>
   </si>
   <si>
-    <t>極圏</t>
-  </si>
-  <si>
-    <t>ウカムルバスの討伐</t>
-  </si>
-  <si>
-    <t>ウカムルバスの顎と背中破壊</t>
+    <t>극천으로부터 온, 무너뜨린 신</t>
+  </si>
+  <si>
+    <t>극권(極圏)</t>
+  </si>
+  <si>
+    <t>우캄룸바스(ウカムルバス) 토벌</t>
+  </si>
+  <si>
+    <t>우캄룸바스(ウカムルバス)의 턱과 등 파괴</t>
   </si>
   <si>
     <t>34800z</t>
@@ -1969,7 +1969,10 @@
     <t>黒蝕竜は禍々しく猛る</t>
   </si>
   <si>
-    <t>ゴア・マガラの翼脚と翼破壊</t>
+    <t>흑식룡은 불길하게 날뛴다</t>
+  </si>
+  <si>
+    <t>고어・마가라(ゴア・マガラ)의 날개 다리와 날개 파괴</t>
   </si>
   <si>
     <t>2600z</t>
@@ -1981,6 +1984,9 @@
     <t>狩人達の究道</t>
   </si>
   <si>
+    <t>사냥꾼들의 구도</t>
+  </si>
+  <si>
     <t>7900z</t>
   </si>
   <si>
@@ -1990,19 +1996,25 @@
     <t>砂漠に散る爆炎の塵</t>
   </si>
   <si>
-    <t>テオ・テスカトルの討伐または撃退</t>
-  </si>
-  <si>
-    <t>テオ・テスカトルの頭部破壊と尻尾切断</t>
+    <t>사막에 흩어지는 폭염의 가루</t>
+  </si>
+  <si>
+    <t>테오・테스카토르(テオ・テスカトル) 토벌 혹은 격퇴</t>
+  </si>
+  <si>
+    <t>테오・테스카토르(テオ・テスカトル)의 머리 파괴와 꼬리 절단</t>
   </si>
   <si>
     <t>天彗龍に目が眩む</t>
   </si>
   <si>
-    <t>バルファルクの討伐または撃退</t>
-  </si>
-  <si>
-    <t>バルファルクの尻尾切断</t>
+    <t>천혜룡에 눈이 멀다</t>
+  </si>
+  <si>
+    <t>발파르크(バルファルク) 토벌 혹은 격퇴</t>
+  </si>
+  <si>
+    <t>발파르크(バルファルク)의 꼬리 절단</t>
   </si>
   <si>
     <t>28200z</t>
@@ -2011,25 +2023,22 @@
     <t>角竜怒涛</t>
   </si>
   <si>
-    <t>旧砂漠</t>
-  </si>
-  <si>
-    <t>ディアブロス１頭の捕獲</t>
-  </si>
-  <si>
-    <t>ディアブロスの背中破壊</t>
+    <t>각룡노도</t>
+  </si>
+  <si>
+    <t>디아블로스(ディアブロス) 1마리 포획</t>
+  </si>
+  <si>
+    <t>디아블로스(ディアブロス)의 등 파괴</t>
   </si>
   <si>
     <t>犯人は黒狼鳥</t>
   </si>
   <si>
-    <t>古代林</t>
-  </si>
-  <si>
-    <t>イャンガルルガ１頭の狩猟</t>
-  </si>
-  <si>
-    <t>イャンガルルガの頭部と翼爪破壊</t>
+    <t>범인은 흑랑룡</t>
+  </si>
+  <si>
+    <t>얀가루루가(イャンガルルガ)의 머리와 날개 발톱 파괴</t>
   </si>
   <si>
     <t>19500z</t>
@@ -2038,22 +2047,22 @@
     <t>所により獰猛なセルレギオス</t>
   </si>
   <si>
-    <t>セルレギオス１頭の狩猟</t>
-  </si>
-  <si>
-    <t>セルレギオスの角と翼破壊</t>
+    <t>장소에 따라 영맹한 셀레기오스</t>
+  </si>
+  <si>
+    <t>셀레기오스(セルレギオス) 1마리 수렵</t>
+  </si>
+  <si>
+    <t>셀레기오스(セルレギオス)의 뿔과 날개 파괴</t>
   </si>
   <si>
     <t>沼地の冒険</t>
   </si>
   <si>
-    <t>沼地</t>
-  </si>
-  <si>
-    <t>グラビモス１頭の狩猟</t>
-  </si>
-  <si>
-    <t>グラビモスの頭部と翼破壊</t>
+    <t>늪지의 모험</t>
+  </si>
+  <si>
+    <t>그라비모스(グラビモス)의 머리와 날개 파괴</t>
   </si>
   <si>
     <t>2500z</t>
@@ -2065,19 +2074,22 @@
     <t>財宝は爆炎の中に</t>
   </si>
   <si>
-    <t>テオ・テスカトルの頭部と翼爪破壊</t>
+    <t>재보는 폭염 속에</t>
+  </si>
+  <si>
+    <t>테오・테스카토르(テオ・テスカトル)의 머리와 양발톱 파괴</t>
   </si>
   <si>
     <t>夜空に浮かぶ銀の太陽</t>
   </si>
   <si>
-    <t>渓流</t>
-  </si>
-  <si>
-    <t>リオレウス希少種１頭の狩猟</t>
-  </si>
-  <si>
-    <t>リオレウス希少種の頭部破壊と尻尾切断</t>
+    <t>밤하늘에 뜬 은의 태앙</t>
+  </si>
+  <si>
+    <t>리오레우스 희소종(リオレウス希少種) 1마리 수렵</t>
+  </si>
+  <si>
+    <t>리오레우스 희소종(リオレウス希少種)의 머리 파괴와 꼬리 절단</t>
   </si>
   <si>
     <t>41100z</t>
@@ -2086,15 +2098,18 @@
     <t>騎士と氷海の決闘</t>
   </si>
   <si>
-    <t>ベリオロス１頭の狩猟</t>
-  </si>
-  <si>
-    <t>ベリオロスの頭部と棘破壊</t>
+    <t>기사와 빙해와 결전</t>
+  </si>
+  <si>
+    <t>베리오로스(ベリオロス)의 머리와 가시 파괴</t>
   </si>
   <si>
     <t>風薫る密林</t>
   </si>
   <si>
+    <t>훈풍의 밀림</t>
+  </si>
+  <si>
     <t>4000z</t>
   </si>
   <si>
@@ -2104,54 +2119,75 @@
     <t>轟竜の軌跡を追いかけて</t>
   </si>
   <si>
-    <t>ティガレックス１頭の狩猟</t>
-  </si>
-  <si>
-    <t>ティガレックスの爪破壊</t>
+    <t>굉룡의 궤적을 뒤쫓아</t>
+  </si>
+  <si>
+    <t>티가렉스(ティガレックス) 1마리 수렵</t>
+  </si>
+  <si>
+    <t>티가렉스(ティガレックス)의 발톱 파괴</t>
   </si>
   <si>
     <t>小山も陽気に誘われて</t>
   </si>
   <si>
-    <t>ドボルベルク１頭の狩猟</t>
-  </si>
-  <si>
-    <t>ドボルベルクの尻尾破壊</t>
+    <t>작은 산도 좋은 날씨에 이끌려</t>
+  </si>
+  <si>
+    <t>도볼베르크(ドボルベルク) 1마리 수렵</t>
+  </si>
+  <si>
+    <t>도볼베르크(ドボルベルク)의 꼬리 파괴</t>
   </si>
   <si>
     <t>鎧竜の背中破壊に挑戦！</t>
   </si>
   <si>
-    <t>グラビモスの背中破壊</t>
+    <t>개룡의 등 파괴에 도전!</t>
+  </si>
+  <si>
+    <t>그라비모스(グラビモス)의 등 파괴</t>
   </si>
   <si>
     <t>天を廻りしその果てに…</t>
   </si>
   <si>
-    <t>禁足地</t>
-  </si>
-  <si>
-    <t>シャガルマガラの討伐</t>
-  </si>
-  <si>
-    <t>シャガルマガラの角と翼脚破壊</t>
+    <t>하늘을 돈 그 말로에...</t>
+  </si>
+  <si>
+    <t>금족지(禁足地)</t>
+  </si>
+  <si>
+    <t>샤갈마가라(シャガルマガラ)の討伐</t>
+  </si>
+  <si>
+    <t>샤갈마가라(シャガルマガラ)의 뿔과 날개 다리 파괴</t>
   </si>
   <si>
     <t>死神は鎧をまとう</t>
   </si>
   <si>
-    <t>グラビモス１頭とネルスキュラ１匹の狩猟</t>
-  </si>
-  <si>
-    <t>乗りによるダウンを３回成功</t>
+    <t>사신은 갑옷을 두르다</t>
+  </si>
+  <si>
+    <t>그라비모스(グラビモス) 1마리와 네르스큐라(ネルスキュラ) 1마리 수렵</t>
+  </si>
+  <si>
+    <t>단차에 의한 다운을３회 성공</t>
   </si>
   <si>
     <t>モンスターニャンターＸＸ</t>
   </si>
   <si>
+    <t>몬스터 냥타 XX</t>
+  </si>
+  <si>
     <t>古代林の陰謀</t>
   </si>
   <si>
+    <t>고대림의 음모</t>
+  </si>
+  <si>
     <t>5300z</t>
   </si>
   <si>
@@ -2161,22 +2197,28 @@
     <t>絆の証！孤島の大決戦</t>
   </si>
   <si>
+    <t>인연의 증거! 고도의 대결전</t>
+  </si>
+  <si>
     <t>31200z</t>
   </si>
   <si>
     <t>巨獣の進攻</t>
   </si>
   <si>
-    <t>ガムート１頭の狩猟</t>
-  </si>
-  <si>
-    <t>ガムートの頭部と鼻破壊</t>
+    <t>거수의 진격</t>
+  </si>
+  <si>
+    <t>가무토(ガムート)의 머리와 코 파괴</t>
   </si>
   <si>
     <t>戈と槌は相容れず</t>
   </si>
   <si>
-    <t>アグナコトル１頭とドボルベルク１頭の狩猟</t>
+    <t>창과 망치는 서로 용납하지 않고</t>
+  </si>
+  <si>
+    <t>아그나코토루(アグナコトル) 1마리와 도볼베르크(ドボルベルク) 1마리 수렵</t>
   </si>
   <si>
     <t>30600z</t>
@@ -2185,10 +2227,13 @@
     <t>暴飲暴食ご用心</t>
   </si>
   <si>
-    <t>イビルジョー１頭の狩猟</t>
-  </si>
-  <si>
-    <t>イビルジョーの頭部破壊</t>
+    <t>폭음폭식에 주의</t>
+  </si>
+  <si>
+    <t>이빌죠(イビルジョー) 1마리 수렵</t>
+  </si>
+  <si>
+    <t>이빌죠(イビルジョー)의 머리 파괴</t>
   </si>
   <si>
     <t>27000z</t>
@@ -2197,46 +2242,58 @@
     <t>戦慄の遺群嶺</t>
   </si>
   <si>
+    <t>전율의 유군령</t>
+  </si>
+  <si>
     <t>46200z</t>
   </si>
   <si>
     <t>徹甲虫と夫婦の絆</t>
   </si>
   <si>
-    <t>アルセルタス１匹の狩猟</t>
+    <t>철갑충과 부부의 인연</t>
   </si>
   <si>
     <t>森丘からの伝書</t>
   </si>
   <si>
+    <t>숲과언덕으로부터의 전서</t>
+  </si>
+  <si>
     <t>砂漠の死闘と挑戦</t>
   </si>
   <si>
-    <t>ディアブロス１頭の狩猟</t>
-  </si>
-  <si>
-    <t>ディアブロスの両角と背中破壊</t>
+    <t>사막의 사투와 도전</t>
+  </si>
+  <si>
+    <t>디아블로스(ディアブロス) 1마리 수렵</t>
+  </si>
+  <si>
+    <t>디아블로스(ディアブロス)의 양뿔과 등 파괴</t>
   </si>
   <si>
     <t>獰猛な海の王者は武器の素</t>
   </si>
   <si>
-    <t>ラギアクルス１頭の狩猟</t>
-  </si>
-  <si>
-    <t>ラギアクルスの胸部破壊と尻尾切断</t>
+    <t>영맹한 바다의 왕은 무기의 소재</t>
+  </si>
+  <si>
+    <t>라기아크루스(ラギアクルス)의 가슴 파괴와 꼬리 절단</t>
   </si>
   <si>
     <t>天を貫く凶星</t>
   </si>
   <si>
+    <t>하늘을 꿰뚫는 흉성</t>
+  </si>
+  <si>
     <t>斬鉄の剣、不壊の鎧</t>
   </si>
   <si>
-    <t>ディノバルド１頭とグラビモス１頭の狩猟</t>
-  </si>
-  <si>
-    <t xml:space="preserve">竜の大粒ナミダ１個の納品 </t>
+    <t>참철의 검, 불괴의 갑옷</t>
+  </si>
+  <si>
+    <t>디노발드(ディノバルド)１頭と그라비모스(グラビモス) 1마리 수렵</t>
   </si>
   <si>
     <t>29700z</t>
@@ -2245,193 +2302,259 @@
     <t>スーパーソニック</t>
   </si>
   <si>
-    <t>バルファルクの翼破壊</t>
+    <t>슈퍼 소닉</t>
+  </si>
+  <si>
+    <t>발파르크(バルファルク)의 날개 파괴</t>
   </si>
   <si>
     <t>金色に染まる</t>
   </si>
   <si>
-    <t>遺跡平原</t>
+    <t>금빛으로 물들다</t>
   </si>
   <si>
     <t>シャル・ウィ・ダンス？</t>
   </si>
   <si>
-    <t>タマミツネ１頭の狩猟</t>
-  </si>
-  <si>
-    <t>タマミツネの頭部破壊と尻尾切断</t>
+    <t>쉘・위・댄스?</t>
+  </si>
+  <si>
+    <t>타마미츠네(タマミツネ)의 머리 파괴와 꼬리 절단</t>
   </si>
   <si>
     <t>吹雪を呼ぶ者</t>
   </si>
   <si>
-    <t>クシャルダオラの討伐または撃退</t>
-  </si>
-  <si>
-    <t>クシャルダオラの頭部と翼破壊</t>
+    <t>눈보라를 부르는 자</t>
+  </si>
+  <si>
+    <t>쿠샬다오라(クシャルダオラ) 토벌 혹은 격퇴</t>
+  </si>
+  <si>
+    <t>쿠샬다오라(クシャルダオラ)의 머리와 날개 파괴</t>
   </si>
   <si>
     <t>孤島で遭遇！獰猛な雷狼竜</t>
   </si>
   <si>
-    <t>ジンオウガ１頭の狩猟</t>
-  </si>
-  <si>
-    <t>ジンオウガの頭部と前脚破壊</t>
+    <t>고도에서 조우! 영맹한 뇌랑룡</t>
+  </si>
+  <si>
+    <t>진오우가(ジンオウガ)의 머리와 앞다리 파괴</t>
   </si>
   <si>
     <t>雪山からの救援要請</t>
   </si>
   <si>
-    <t>ラージャンの尻尾破壊</t>
+    <t>설산으로부터의 구원요청</t>
+  </si>
+  <si>
+    <t>라쟌(ラージャン)의 꼬리 파괴</t>
   </si>
   <si>
     <t>天を舞う白銀</t>
   </si>
   <si>
-    <t>リオレウス希少種の翼と背中破壊</t>
+    <t>하늘을 나는 백은</t>
+  </si>
+  <si>
+    <t>리오레우스 희소종(リオレウス希少種)의 날개와 등 파괴</t>
   </si>
   <si>
     <t>遺群嶺での攻防</t>
   </si>
   <si>
-    <t>イビルジョーの頭部破壊と尻尾切断</t>
+    <t>유군령에서의 공방</t>
+  </si>
+  <si>
+    <t>이빌죠(イビルジョー)의 머리 파괴와 꼬리 절단</t>
   </si>
   <si>
     <t>狩人のための舞台～古代林～</t>
   </si>
   <si>
-    <t>リオレイア希少種の頭部破壊と尻尾切断</t>
+    <t>사냥꾼들을 위한 무대 ~고대림~</t>
+  </si>
+  <si>
+    <t>리오레이아 희소종(リオレイア希少種)의 머리 파괴와 꼬리 절단</t>
   </si>
   <si>
     <t>呼び合う太陽と月</t>
   </si>
   <si>
+    <t>서로 부르는 태양과 달</t>
+  </si>
+  <si>
     <t>48000z</t>
   </si>
   <si>
     <t>砂上に見ゆるは猛き双角</t>
   </si>
   <si>
-    <t>ディアブロスの両角破壊</t>
+    <t>모래 위에 보이는것은 사나운 쌍각</t>
+  </si>
+  <si>
+    <t>디아블로스(ディアブロス)의 양뿔 파괴</t>
   </si>
   <si>
     <t>禍は鋼鉄よりも硬し</t>
   </si>
   <si>
-    <t>クシャルダオラの頭部破壊と尻尾切断</t>
+    <t>재앙은 강철보다도 단단하다</t>
+  </si>
+  <si>
+    <t>쿠샬다오라(クシャルダオラ)의 머리 파괴와 꼬리 절단</t>
   </si>
   <si>
     <t>千刃は刀よりも鋭く</t>
   </si>
   <si>
-    <t>セルレギオスの角破壊</t>
+    <t>천인은 칼보다도 날카롭다</t>
+  </si>
+  <si>
+    <t>셀레기오스(セルレギオス)의 뿔 파괴</t>
   </si>
   <si>
     <t>焦電</t>
   </si>
   <si>
-    <t>ライゼクス１頭の狩猟</t>
-  </si>
-  <si>
-    <t>ライゼクスのトサカと翼爪破壊</t>
+    <t>초전</t>
+  </si>
+  <si>
+    <t>라이젝스(ライゼクス)의 볏과 날개 발톱 파괴</t>
   </si>
   <si>
     <t>イビルジョーの狩猟</t>
   </si>
   <si>
-    <t>イビルジョーの尻尾切断</t>
+    <t>이빌죠 수렵</t>
+  </si>
+  <si>
+    <t>이빌죠(イビルジョー)의 꼬리 절단</t>
   </si>
   <si>
     <t>起源にして、頂点</t>
   </si>
   <si>
-    <t>アカムトルムの討伐</t>
-  </si>
-  <si>
-    <t>アカムトルムの頭部と背中破壊</t>
+    <t>기원이자, 정점</t>
+  </si>
+  <si>
+    <t>아캄토룸(アカムトルム) 토벌</t>
+  </si>
+  <si>
+    <t>아캄토룸(アカムトルム)의 머리와 등 파괴</t>
   </si>
   <si>
     <t>全てを奪い去る嵐</t>
   </si>
   <si>
-    <t>霊峰</t>
-  </si>
-  <si>
-    <t>アマツマガツチの討伐</t>
-  </si>
-  <si>
-    <t>アマツマガツチの頭部と背中破壊</t>
+    <t>모든것을 앗아가는 폭풍</t>
+  </si>
+  <si>
+    <t>영봉(霊峰)</t>
+  </si>
+  <si>
+    <t>아마츠마가츠치(アマツマガツチ) 토벌</t>
+  </si>
+  <si>
+    <t>아마츠마가츠치(アマツマガツチ)의 머리와 등 파괴</t>
   </si>
   <si>
     <t>砂漠の死闘と未来</t>
   </si>
   <si>
+    <t>사막의 사투와 미래</t>
+  </si>
+  <si>
     <t>骸まとう龍</t>
   </si>
   <si>
-    <t>竜ノ墓場</t>
-  </si>
-  <si>
-    <t>オストガロアの討伐</t>
-  </si>
-  <si>
-    <t>オストガロアの左右噴出孔破壊</t>
+    <t>뼈를 두른 용</t>
+  </si>
+  <si>
+    <t>용의 무덤(竜ノ墓場)</t>
+  </si>
+  <si>
+    <t>오스트가로아(オストガロア) 토벌</t>
+  </si>
+  <si>
+    <t>오스트가로아(オストガロア)의 좌우 분출 구멍 파괴</t>
   </si>
   <si>
     <t>天彗龍流狩人道場</t>
   </si>
   <si>
-    <t>いにしえの龍秘宝１個の納品</t>
+    <t>천혜룡류 사냥꾼 도장</t>
+  </si>
+  <si>
+    <t>고대의 용비보(いにしえの龍秘宝) 1개 납품</t>
   </si>
   <si>
     <t>無心にて森羅万象を断つ</t>
   </si>
   <si>
-    <t>ディノバルド１頭の狩猟</t>
-  </si>
-  <si>
-    <t>ディノバルドの背中破壊と尻尾切断</t>
+    <t>무심으로 삼라만상을 자른다</t>
+  </si>
+  <si>
+    <t>디노발드(ディノバルド)의 등 파괴와 꼬리 절단</t>
   </si>
   <si>
     <t>轟々たる罠</t>
   </si>
   <si>
-    <t>ティガレックスの頭部破壊と尻尾切断</t>
+    <t>요란한 함정</t>
+  </si>
+  <si>
+    <t>티가렉스(ティガレックス)의 머리 파괴와 꼬리 절단</t>
   </si>
   <si>
     <t>光る粘菌のナゾを追え</t>
   </si>
   <si>
-    <t>ブラキディオス１頭の捕獲</t>
+    <t>빛나는 점균의 수수께끼를 쫓아</t>
+  </si>
+  <si>
+    <t>브라키디오스(ブラキディオス) 1마리 포획</t>
   </si>
   <si>
     <t>この先、千刃竜以外立入禁止</t>
   </si>
   <si>
-    <t>セルレギオスの脚破壊</t>
+    <t>이 앞, 천인룡 이외 출입 금지</t>
+  </si>
+  <si>
+    <t>셀레기오스(セルレギオス)의 다리 파괴</t>
   </si>
   <si>
     <t>海竜の頭部破壊に挑戦！</t>
   </si>
   <si>
-    <t>ラギアクルスの頭部破壊</t>
+    <t>해룡의 머리 파괴에 도전!</t>
   </si>
   <si>
     <t>虚空より現われし者</t>
   </si>
   <si>
-    <t>オオナズチの角と翼破壊</t>
+    <t>허공으로부터 나타난 자</t>
+  </si>
+  <si>
+    <t>오나즈치(オオナズチ)の토벌 혹은 격퇴</t>
+  </si>
+  <si>
+    <t>오나즈치(オオナズチ)의 뿔과 날개 파괴</t>
   </si>
   <si>
     <t>溶岩島で爆ぜる砕光</t>
   </si>
   <si>
-    <t>ブラキディオスの討伐</t>
-  </si>
-  <si>
-    <t>ブラキディオスの頭部破壊</t>
+    <t>용암도에서 터지는 쇄광</t>
+  </si>
+  <si>
+    <t>브라키디오스(ブラキディオス) 토벌</t>
+  </si>
+  <si>
+    <t>브라키디오스(ブラキディオス)의 머리 파괴</t>
   </si>
   <si>
     <t>3400z</t>
@@ -2443,49 +2566,64 @@
     <t>原生林にて呻くは渾沌の竜</t>
   </si>
   <si>
-    <t>ゴア・マガラの左翼脚破壊</t>
+    <t>원시림에서 신음하는 혼돈의 용</t>
+  </si>
+  <si>
+    <t>고어・마가라(ゴア・マガラ)의 좌측 날개 다리 파괴</t>
   </si>
   <si>
     <t>火山のすばらしい岩</t>
   </si>
   <si>
-    <t>リオレウス１頭の狩猟</t>
-  </si>
-  <si>
-    <t>リオレウスの頭部と翼破壊</t>
+    <t>화산의 굉장한 바위</t>
+  </si>
+  <si>
+    <t>리오레우스(リオレウス)의 머리와 날개 파괴</t>
   </si>
   <si>
     <t>マグマまといし竜</t>
   </si>
   <si>
-    <t>アグナコトル１頭の狩猟</t>
-  </si>
-  <si>
-    <t>アグナコトルの胸部破壊</t>
+    <t>마그마를 두른 용</t>
+  </si>
+  <si>
+    <t>아그나코토루(アグナコトル) 1마리 수렵</t>
+  </si>
+  <si>
+    <t>아그나코토루(アグナコトル)의 가슴 파괴</t>
   </si>
   <si>
     <t>天地が焔に染まるとき</t>
   </si>
   <si>
-    <t>リオレウス１頭とリオレイア１頭の狩猟</t>
+    <t>천지가 불꽃에 물드는 때</t>
   </si>
   <si>
     <t>氷海を爆走、暴走轟竜！</t>
   </si>
   <si>
-    <t>ティガレックスの頭部破壊</t>
+    <t>빙해를 폭주, 폭주굉룡!</t>
+  </si>
+  <si>
+    <t>티가렉스(ティガレックス)의 머리 파괴</t>
   </si>
   <si>
     <t>炎戈竜は地底で吠える</t>
   </si>
   <si>
-    <t>アグナコトルの頭部と胸部破壊</t>
+    <t>염과룡은 지저에서 울부짖는다</t>
+  </si>
+  <si>
+    <t>아그나코토루(アグナコトル)의 머리와 가슴 파괴</t>
   </si>
   <si>
     <t>絆の証！闘技場の大決戦</t>
   </si>
   <si>
-    <t>乗りによるダウンを５回成功</t>
+    <t>인연의 증거! 투기장의 대결전</t>
+  </si>
+  <si>
+    <t>단차에 의한 다운을５회 성공</t>
   </si>
   <si>
     <t>57000z</t>
@@ -2494,49 +2632,70 @@
     <t>火山の脅威・ブラキディオス</t>
   </si>
   <si>
-    <t>ブラキディオスの前脚破壊</t>
+    <t>화산의 위협・브라키디오스</t>
+  </si>
+  <si>
+    <t>브라키디오스(ブラキディオス)의 앞다리 파괴</t>
   </si>
   <si>
     <t>我怒る、ゆえに我在り</t>
   </si>
   <si>
-    <t>ラージャンの角と尻尾破壊</t>
+    <t>나는 분노한다, 고로 나는 존재한다</t>
+  </si>
+  <si>
+    <t>라쟌(ラージャン)의 뿔과 꼬리 파괴</t>
   </si>
   <si>
     <t>神への抵抗</t>
   </si>
   <si>
-    <t>アルバトリオンの討伐</t>
-  </si>
-  <si>
-    <t>アルバトリオンの角と翼破壊</t>
+    <t>신을 향한 저항</t>
+  </si>
+  <si>
+    <t>알바트리온(アルバトリオン) 토벌</t>
+  </si>
+  <si>
+    <t>알바트리온(アルバトリオン)의 뿔과 날개 파괴</t>
   </si>
   <si>
     <t>領主の懇願～尾槌竜篇～</t>
   </si>
   <si>
-    <t>ドボルベルクの角と尻尾破壊</t>
+    <t>영주의 간원 ~미추룡편~</t>
+  </si>
+  <si>
+    <t>도볼베르크(ドボルベルク)의 뿔과 꼬리 파괴</t>
   </si>
   <si>
     <t>蠢く墟城</t>
   </si>
   <si>
-    <t>旧砦跡</t>
-  </si>
-  <si>
-    <t xml:space="preserve">アトラル・カの討伐 </t>
+    <t>꿈틀거리는 허성</t>
+  </si>
+  <si>
+    <t>구채적(旧砦跡)</t>
+  </si>
+  <si>
+    <t>아트랄・카(アトラル・カ) 토벌 </t>
   </si>
   <si>
     <t>伝説の黒龍</t>
   </si>
   <si>
-    <t>シュレイド城</t>
+    <t>전설의 흑룡</t>
+  </si>
+  <si>
+    <t>슈레이드성(シュレイド城)</t>
   </si>
   <si>
     <t>祖龍</t>
   </si>
   <si>
-    <t>ミラルーツの討伐または撃退</t>
+    <t>조룡</t>
+  </si>
+  <si>
+    <t>밀라루츠(ミラルーツ) 토벌 혹은 격퇴</t>
   </si>
 </sst>
 </file>
@@ -2915,8 +3074,8 @@
   <dimension ref="A1:J231"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
-      <pane ySplit="1" topLeftCell="A132" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D145" sqref="D145"/>
+      <pane ySplit="1" topLeftCell="B200" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G206" sqref="G206"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -7511,26 +7670,29 @@
       <c r="A146" t="s">
         <v>580</v>
       </c>
+      <c r="B146" t="s">
+        <v>581</v>
+      </c>
       <c r="C146" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
       <c r="D146" t="s">
-        <v>582</v>
+        <v>119</v>
       </c>
       <c r="E146" t="s">
         <v>14</v>
       </c>
       <c r="F146" t="s">
+        <v>297</v>
+      </c>
+      <c r="G146" t="s">
         <v>583</v>
       </c>
-      <c r="G146" t="s">
+      <c r="H146" t="s">
         <v>584</v>
       </c>
-      <c r="H146" t="s">
+      <c r="I146" t="s">
         <v>585</v>
-      </c>
-      <c r="I146" t="s">
-        <v>586</v>
       </c>
       <c r="J146" t="s">
         <v>51</v>
@@ -7538,28 +7700,31 @@
     </row>
     <row r="147" spans="1:10">
       <c r="A147" t="s">
+        <v>586</v>
+      </c>
+      <c r="B147" t="s">
         <v>587</v>
       </c>
       <c r="C147" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
       <c r="D147" t="s">
+        <v>45</v>
+      </c>
+      <c r="E147" t="s">
+        <v>14</v>
+      </c>
+      <c r="F147" t="s">
         <v>588</v>
-      </c>
-      <c r="E147" t="s">
-        <v>14</v>
-      </c>
-      <c r="F147" t="s">
-        <v>589</v>
       </c>
       <c r="G147" t="s">
         <v>16</v>
       </c>
       <c r="H147" t="s">
+        <v>589</v>
+      </c>
+      <c r="I147" t="s">
         <v>590</v>
-      </c>
-      <c r="I147" t="s">
-        <v>591</v>
       </c>
       <c r="J147" t="s">
         <v>23</v>
@@ -7567,51 +7732,57 @@
     </row>
     <row r="148" spans="1:10">
       <c r="A148" t="s">
+        <v>591</v>
+      </c>
+      <c r="B148" t="s">
         <v>592</v>
       </c>
       <c r="C148" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
       <c r="D148" t="s">
+        <v>296</v>
+      </c>
+      <c r="E148" t="s">
+        <v>14</v>
+      </c>
+      <c r="F148" t="s">
         <v>593</v>
       </c>
-      <c r="E148" t="s">
-        <v>14</v>
-      </c>
-      <c r="F148" t="s">
+      <c r="G148" t="s">
         <v>594</v>
       </c>
-      <c r="G148" t="s">
+      <c r="H148" t="s">
         <v>595</v>
       </c>
-      <c r="H148" t="s">
+      <c r="I148" t="s">
         <v>596</v>
       </c>
-      <c r="I148" t="s">
+      <c r="J148" t="s">
         <v>597</v>
-      </c>
-      <c r="J148" t="s">
-        <v>598</v>
       </c>
     </row>
     <row r="149" spans="1:10">
       <c r="A149" t="s">
+        <v>598</v>
+      </c>
+      <c r="B149" t="s">
         <v>599</v>
       </c>
       <c r="C149" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
       <c r="D149" t="s">
+        <v>21</v>
+      </c>
+      <c r="E149" t="s">
+        <v>14</v>
+      </c>
+      <c r="F149" t="s">
+        <v>447</v>
+      </c>
+      <c r="G149" t="s">
         <v>600</v>
-      </c>
-      <c r="E149" t="s">
-        <v>14</v>
-      </c>
-      <c r="F149" t="s">
-        <v>601</v>
-      </c>
-      <c r="G149" t="s">
-        <v>602</v>
       </c>
       <c r="H149" t="s">
         <v>406</v>
@@ -7625,28 +7796,31 @@
     </row>
     <row r="150" spans="1:10">
       <c r="A150" t="s">
+        <v>601</v>
+      </c>
+      <c r="B150" t="s">
+        <v>602</v>
+      </c>
+      <c r="C150" t="s">
+        <v>582</v>
+      </c>
+      <c r="D150" t="s">
+        <v>366</v>
+      </c>
+      <c r="E150" t="s">
+        <v>14</v>
+      </c>
+      <c r="F150" t="s">
+        <v>367</v>
+      </c>
+      <c r="G150" t="s">
         <v>603</v>
-      </c>
-      <c r="C150" t="s">
-        <v>581</v>
-      </c>
-      <c r="D150" t="s">
-        <v>604</v>
-      </c>
-      <c r="E150" t="s">
-        <v>14</v>
-      </c>
-      <c r="F150" t="s">
-        <v>605</v>
-      </c>
-      <c r="G150" t="s">
-        <v>606</v>
       </c>
       <c r="H150" t="s">
         <v>69</v>
       </c>
       <c r="I150" t="s">
-        <v>607</v>
+        <v>604</v>
       </c>
       <c r="J150" t="s">
         <v>227</v>
@@ -7654,28 +7828,31 @@
     </row>
     <row r="151" spans="1:10">
       <c r="A151" t="s">
+        <v>605</v>
+      </c>
+      <c r="B151" t="s">
+        <v>606</v>
+      </c>
+      <c r="C151" t="s">
+        <v>582</v>
+      </c>
+      <c r="D151" t="s">
+        <v>158</v>
+      </c>
+      <c r="E151" t="s">
+        <v>14</v>
+      </c>
+      <c r="F151" t="s">
+        <v>297</v>
+      </c>
+      <c r="G151" t="s">
+        <v>361</v>
+      </c>
+      <c r="H151" t="s">
+        <v>607</v>
+      </c>
+      <c r="I151" t="s">
         <v>608</v>
-      </c>
-      <c r="C151" t="s">
-        <v>581</v>
-      </c>
-      <c r="D151" t="s">
-        <v>609</v>
-      </c>
-      <c r="E151" t="s">
-        <v>14</v>
-      </c>
-      <c r="F151" t="s">
-        <v>583</v>
-      </c>
-      <c r="G151" t="s">
-        <v>584</v>
-      </c>
-      <c r="H151" t="s">
-        <v>610</v>
-      </c>
-      <c r="I151" t="s">
-        <v>611</v>
       </c>
       <c r="J151" t="s">
         <v>51</v>
@@ -7683,28 +7860,31 @@
     </row>
     <row r="152" spans="1:10">
       <c r="A152" t="s">
+        <v>609</v>
+      </c>
+      <c r="B152" t="s">
+        <v>610</v>
+      </c>
+      <c r="C152" t="s">
+        <v>582</v>
+      </c>
+      <c r="D152" t="s">
+        <v>175</v>
+      </c>
+      <c r="E152" t="s">
+        <v>14</v>
+      </c>
+      <c r="F152" t="s">
+        <v>611</v>
+      </c>
+      <c r="G152" t="s">
         <v>612</v>
-      </c>
-      <c r="C152" t="s">
-        <v>581</v>
-      </c>
-      <c r="D152" t="s">
-        <v>613</v>
-      </c>
-      <c r="E152" t="s">
-        <v>14</v>
-      </c>
-      <c r="F152" t="s">
-        <v>614</v>
-      </c>
-      <c r="G152" t="s">
-        <v>615</v>
       </c>
       <c r="H152" t="s">
         <v>116</v>
       </c>
       <c r="I152" t="s">
-        <v>616</v>
+        <v>613</v>
       </c>
       <c r="J152" t="s">
         <v>227</v>
@@ -7712,28 +7892,31 @@
     </row>
     <row r="153" spans="1:10">
       <c r="A153" t="s">
-        <v>617</v>
+        <v>614</v>
+      </c>
+      <c r="B153" t="s">
+        <v>615</v>
       </c>
       <c r="C153" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
       <c r="D153" t="s">
-        <v>618</v>
+        <v>616</v>
       </c>
       <c r="E153" t="s">
         <v>570</v>
       </c>
       <c r="F153" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="G153" t="s">
         <v>16</v>
       </c>
       <c r="H153" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="I153" t="s">
-        <v>620</v>
+        <v>618</v>
       </c>
       <c r="J153" t="s">
         <v>23</v>
@@ -7741,22 +7924,25 @@
     </row>
     <row r="154" spans="1:10">
       <c r="A154" t="s">
+        <v>619</v>
+      </c>
+      <c r="B154" t="s">
+        <v>620</v>
+      </c>
+      <c r="C154" t="s">
+        <v>582</v>
+      </c>
+      <c r="D154" t="s">
+        <v>236</v>
+      </c>
+      <c r="E154" t="s">
+        <v>14</v>
+      </c>
+      <c r="F154" t="s">
         <v>621</v>
       </c>
-      <c r="C154" t="s">
-        <v>581</v>
-      </c>
-      <c r="D154" t="s">
+      <c r="G154" t="s">
         <v>622</v>
-      </c>
-      <c r="E154" t="s">
-        <v>14</v>
-      </c>
-      <c r="F154" t="s">
-        <v>623</v>
-      </c>
-      <c r="G154" t="s">
-        <v>624</v>
       </c>
       <c r="H154" t="s">
         <v>478</v>
@@ -7770,57 +7956,63 @@
     </row>
     <row r="155" spans="1:10">
       <c r="A155" t="s">
+        <v>623</v>
+      </c>
+      <c r="B155" t="s">
+        <v>624</v>
+      </c>
+      <c r="C155" t="s">
+        <v>582</v>
+      </c>
+      <c r="D155" t="s">
+        <v>175</v>
+      </c>
+      <c r="E155" t="s">
+        <v>14</v>
+      </c>
+      <c r="F155" t="s">
         <v>625</v>
       </c>
-      <c r="C155" t="s">
-        <v>581</v>
-      </c>
-      <c r="D155" t="s">
-        <v>613</v>
-      </c>
-      <c r="E155" t="s">
-        <v>14</v>
-      </c>
-      <c r="F155" t="s">
+      <c r="G155" t="s">
         <v>626</v>
       </c>
-      <c r="G155" t="s">
+      <c r="H155" t="s">
         <v>627</v>
       </c>
-      <c r="H155" t="s">
+      <c r="I155" t="s">
         <v>628</v>
       </c>
-      <c r="I155" t="s">
-        <v>629</v>
-      </c>
       <c r="J155" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
     </row>
     <row r="156" spans="1:10">
       <c r="A156" t="s">
+        <v>629</v>
+      </c>
+      <c r="B156" t="s">
         <v>630</v>
       </c>
       <c r="C156" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
       <c r="D156" t="s">
+        <v>13</v>
+      </c>
+      <c r="E156" t="s">
+        <v>14</v>
+      </c>
+      <c r="F156" t="s">
+        <v>297</v>
+      </c>
+      <c r="G156" t="s">
+        <v>361</v>
+      </c>
+      <c r="H156" t="s">
         <v>631</v>
       </c>
-      <c r="E156" t="s">
-        <v>14</v>
-      </c>
-      <c r="F156" t="s">
-        <v>583</v>
-      </c>
-      <c r="G156" t="s">
-        <v>584</v>
-      </c>
-      <c r="H156" t="s">
+      <c r="I156" t="s">
         <v>632</v>
-      </c>
-      <c r="I156" t="s">
-        <v>633</v>
       </c>
       <c r="J156" t="s">
         <v>51</v>
@@ -7828,28 +8020,31 @@
     </row>
     <row r="157" spans="1:10">
       <c r="A157" t="s">
+        <v>633</v>
+      </c>
+      <c r="B157" t="s">
         <v>634</v>
       </c>
       <c r="C157" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
       <c r="D157" t="s">
-        <v>635</v>
+        <v>55</v>
       </c>
       <c r="E157" t="s">
         <v>570</v>
       </c>
       <c r="F157" t="s">
+        <v>635</v>
+      </c>
+      <c r="G157" t="s">
         <v>636</v>
-      </c>
-      <c r="G157" t="s">
-        <v>637</v>
       </c>
       <c r="H157" t="s">
         <v>116</v>
       </c>
       <c r="I157" t="s">
-        <v>616</v>
+        <v>613</v>
       </c>
       <c r="J157" t="s">
         <v>51</v>
@@ -7857,19 +8052,22 @@
     </row>
     <row r="158" spans="1:10">
       <c r="A158" t="s">
+        <v>637</v>
+      </c>
+      <c r="B158" t="s">
         <v>638</v>
       </c>
       <c r="C158" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
       <c r="D158" t="s">
+        <v>170</v>
+      </c>
+      <c r="E158" t="s">
+        <v>14</v>
+      </c>
+      <c r="F158" t="s">
         <v>639</v>
-      </c>
-      <c r="E158" t="s">
-        <v>14</v>
-      </c>
-      <c r="F158" t="s">
-        <v>640</v>
       </c>
       <c r="G158" t="s">
         <v>16</v>
@@ -7886,22 +8084,25 @@
     </row>
     <row r="159" spans="1:10">
       <c r="A159" t="s">
+        <v>640</v>
+      </c>
+      <c r="B159" t="s">
         <v>641</v>
       </c>
       <c r="C159" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
       <c r="D159" t="s">
-        <v>588</v>
+        <v>45</v>
       </c>
       <c r="E159" t="s">
         <v>14</v>
       </c>
       <c r="F159" t="s">
+        <v>473</v>
+      </c>
+      <c r="G159" t="s">
         <v>642</v>
-      </c>
-      <c r="G159" t="s">
-        <v>643</v>
       </c>
       <c r="H159" t="s">
         <v>362</v>
@@ -7915,10 +8116,13 @@
     </row>
     <row r="160" spans="1:10">
       <c r="A160" t="s">
+        <v>643</v>
+      </c>
+      <c r="B160" t="s">
         <v>644</v>
       </c>
       <c r="C160" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
       <c r="D160" t="s">
         <v>645</v>
@@ -7933,7 +8137,7 @@
         <v>647</v>
       </c>
       <c r="H160" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="I160" t="s">
         <v>648</v>
@@ -7946,26 +8150,29 @@
       <c r="A161" t="s">
         <v>649</v>
       </c>
+      <c r="B161" t="s">
+        <v>650</v>
+      </c>
       <c r="C161" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
       <c r="D161" t="s">
-        <v>600</v>
+        <v>21</v>
       </c>
       <c r="E161" t="s">
         <v>14</v>
       </c>
       <c r="F161" t="s">
-        <v>642</v>
+        <v>473</v>
       </c>
       <c r="G161" t="s">
-        <v>650</v>
+        <v>651</v>
       </c>
       <c r="H161" t="s">
-        <v>651</v>
+        <v>652</v>
       </c>
       <c r="I161" t="s">
-        <v>652</v>
+        <v>653</v>
       </c>
       <c r="J161" t="s">
         <v>227</v>
@@ -7973,28 +8180,31 @@
     </row>
     <row r="162" spans="1:10">
       <c r="A162" t="s">
-        <v>653</v>
+        <v>654</v>
+      </c>
+      <c r="B162" t="s">
+        <v>655</v>
       </c>
       <c r="C162" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
       <c r="D162" t="s">
-        <v>593</v>
+        <v>296</v>
       </c>
       <c r="E162" t="s">
         <v>14</v>
       </c>
       <c r="F162" t="s">
-        <v>583</v>
+        <v>297</v>
       </c>
       <c r="G162" t="s">
         <v>16</v>
       </c>
       <c r="H162" t="s">
-        <v>654</v>
+        <v>656</v>
       </c>
       <c r="I162" t="s">
-        <v>655</v>
+        <v>657</v>
       </c>
       <c r="J162" t="s">
         <v>23</v>
@@ -8002,28 +8212,31 @@
     </row>
     <row r="163" spans="1:10">
       <c r="A163" t="s">
-        <v>656</v>
+        <v>658</v>
+      </c>
+      <c r="B163" t="s">
+        <v>659</v>
       </c>
       <c r="C163" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
       <c r="D163" t="s">
-        <v>631</v>
+        <v>13</v>
       </c>
       <c r="E163" t="s">
         <v>570</v>
       </c>
       <c r="F163" t="s">
-        <v>657</v>
+        <v>660</v>
       </c>
       <c r="G163" t="s">
-        <v>658</v>
+        <v>661</v>
       </c>
       <c r="H163" t="s">
         <v>116</v>
       </c>
       <c r="I163" t="s">
-        <v>616</v>
+        <v>613</v>
       </c>
       <c r="J163" t="s">
         <v>51</v>
@@ -8031,48 +8244,54 @@
     </row>
     <row r="164" spans="1:10">
       <c r="A164" t="s">
-        <v>659</v>
+        <v>662</v>
+      </c>
+      <c r="B164" t="s">
+        <v>663</v>
       </c>
       <c r="C164" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
       <c r="D164" t="s">
-        <v>582</v>
+        <v>119</v>
       </c>
       <c r="E164" t="s">
         <v>14</v>
       </c>
       <c r="F164" t="s">
-        <v>660</v>
+        <v>664</v>
       </c>
       <c r="G164" t="s">
-        <v>661</v>
+        <v>665</v>
       </c>
       <c r="I164" t="s">
-        <v>662</v>
+        <v>666</v>
       </c>
       <c r="J164" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
     </row>
     <row r="165" spans="1:10">
       <c r="A165" t="s">
-        <v>663</v>
+        <v>667</v>
+      </c>
+      <c r="B165" t="s">
+        <v>668</v>
       </c>
       <c r="C165" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
       <c r="D165" t="s">
-        <v>664</v>
+        <v>42</v>
       </c>
       <c r="E165" t="s">
         <v>14</v>
       </c>
       <c r="F165" t="s">
-        <v>665</v>
+        <v>669</v>
       </c>
       <c r="G165" t="s">
-        <v>666</v>
+        <v>670</v>
       </c>
       <c r="H165" t="s">
         <v>478</v>
@@ -8081,33 +8300,36 @@
         <v>479</v>
       </c>
       <c r="J165" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
     </row>
     <row r="166" spans="1:10">
       <c r="A166" t="s">
-        <v>667</v>
+        <v>671</v>
+      </c>
+      <c r="B166" t="s">
+        <v>672</v>
       </c>
       <c r="C166" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
       <c r="D166" t="s">
-        <v>668</v>
+        <v>64</v>
       </c>
       <c r="E166" t="s">
         <v>14</v>
       </c>
       <c r="F166" t="s">
-        <v>669</v>
+        <v>499</v>
       </c>
       <c r="G166" t="s">
-        <v>670</v>
+        <v>673</v>
       </c>
       <c r="H166" t="s">
         <v>299</v>
       </c>
       <c r="I166" t="s">
-        <v>671</v>
+        <v>674</v>
       </c>
       <c r="J166" t="s">
         <v>227</v>
@@ -8115,22 +8337,25 @@
     </row>
     <row r="167" spans="1:10">
       <c r="A167" t="s">
-        <v>672</v>
+        <v>675</v>
+      </c>
+      <c r="B167" t="s">
+        <v>676</v>
       </c>
       <c r="C167" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
       <c r="D167" t="s">
-        <v>664</v>
+        <v>42</v>
       </c>
       <c r="E167" t="s">
         <v>14</v>
       </c>
       <c r="F167" t="s">
-        <v>673</v>
+        <v>677</v>
       </c>
       <c r="G167" t="s">
-        <v>674</v>
+        <v>678</v>
       </c>
       <c r="H167" t="s">
         <v>478</v>
@@ -8144,28 +8369,31 @@
     </row>
     <row r="168" spans="1:10">
       <c r="A168" t="s">
-        <v>675</v>
+        <v>679</v>
+      </c>
+      <c r="B168" t="s">
+        <v>680</v>
       </c>
       <c r="C168" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
       <c r="D168" t="s">
-        <v>676</v>
+        <v>164</v>
       </c>
       <c r="E168" t="s">
         <v>14</v>
       </c>
       <c r="F168" t="s">
-        <v>677</v>
+        <v>578</v>
       </c>
       <c r="G168" t="s">
-        <v>678</v>
+        <v>681</v>
       </c>
       <c r="H168" t="s">
-        <v>679</v>
+        <v>682</v>
       </c>
       <c r="I168" t="s">
-        <v>680</v>
+        <v>683</v>
       </c>
       <c r="J168" t="s">
         <v>227</v>
@@ -8173,25 +8401,28 @@
     </row>
     <row r="169" spans="1:10">
       <c r="A169" t="s">
-        <v>681</v>
+        <v>684</v>
+      </c>
+      <c r="B169" t="s">
+        <v>685</v>
       </c>
       <c r="C169" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
       <c r="D169" t="s">
-        <v>609</v>
+        <v>158</v>
       </c>
       <c r="E169" t="s">
         <v>14</v>
       </c>
       <c r="F169" t="s">
-        <v>657</v>
+        <v>660</v>
       </c>
       <c r="G169" t="s">
-        <v>682</v>
+        <v>686</v>
       </c>
       <c r="I169" t="s">
-        <v>616</v>
+        <v>613</v>
       </c>
       <c r="J169" t="s">
         <v>51</v>
@@ -8199,28 +8430,31 @@
     </row>
     <row r="170" spans="1:10">
       <c r="A170" t="s">
-        <v>683</v>
+        <v>687</v>
+      </c>
+      <c r="B170" t="s">
+        <v>688</v>
       </c>
       <c r="C170" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
       <c r="D170" t="s">
-        <v>684</v>
+        <v>72</v>
       </c>
       <c r="E170" t="s">
         <v>14</v>
       </c>
       <c r="F170" t="s">
-        <v>685</v>
+        <v>689</v>
       </c>
       <c r="G170" t="s">
-        <v>686</v>
+        <v>690</v>
       </c>
       <c r="H170" t="s">
         <v>161</v>
       </c>
       <c r="I170" t="s">
-        <v>687</v>
+        <v>691</v>
       </c>
       <c r="J170" t="s">
         <v>227</v>
@@ -8228,22 +8462,25 @@
     </row>
     <row r="171" spans="1:10">
       <c r="A171" t="s">
-        <v>688</v>
+        <v>692</v>
+      </c>
+      <c r="B171" t="s">
+        <v>693</v>
       </c>
       <c r="C171" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
       <c r="D171" t="s">
-        <v>639</v>
+        <v>170</v>
       </c>
       <c r="E171" t="s">
         <v>14</v>
       </c>
       <c r="F171" t="s">
-        <v>689</v>
+        <v>487</v>
       </c>
       <c r="G171" t="s">
-        <v>690</v>
+        <v>694</v>
       </c>
       <c r="H171" t="s">
         <v>406</v>
@@ -8257,28 +8494,31 @@
     </row>
     <row r="172" spans="1:10">
       <c r="A172" t="s">
-        <v>691</v>
+        <v>695</v>
+      </c>
+      <c r="B172" t="s">
+        <v>696</v>
       </c>
       <c r="C172" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
       <c r="D172" t="s">
-        <v>613</v>
+        <v>175</v>
       </c>
       <c r="E172" t="s">
         <v>14</v>
       </c>
       <c r="F172" t="s">
-        <v>583</v>
+        <v>297</v>
       </c>
       <c r="G172" t="s">
-        <v>584</v>
+        <v>361</v>
       </c>
       <c r="H172" t="s">
-        <v>692</v>
+        <v>697</v>
       </c>
       <c r="I172" t="s">
-        <v>693</v>
+        <v>698</v>
       </c>
       <c r="J172" t="s">
         <v>51</v>
@@ -8286,22 +8526,25 @@
     </row>
     <row r="173" spans="1:10">
       <c r="A173" t="s">
-        <v>694</v>
+        <v>699</v>
+      </c>
+      <c r="B173" t="s">
+        <v>700</v>
       </c>
       <c r="C173" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
       <c r="D173" t="s">
-        <v>600</v>
+        <v>21</v>
       </c>
       <c r="E173" t="s">
         <v>14</v>
       </c>
       <c r="F173" t="s">
-        <v>695</v>
+        <v>701</v>
       </c>
       <c r="G173" t="s">
-        <v>696</v>
+        <v>702</v>
       </c>
       <c r="H173" t="s">
         <v>406</v>
@@ -8310,27 +8553,30 @@
         <v>407</v>
       </c>
       <c r="J173" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
     </row>
     <row r="174" spans="1:10">
       <c r="A174" t="s">
-        <v>697</v>
+        <v>703</v>
+      </c>
+      <c r="B174" t="s">
+        <v>704</v>
       </c>
       <c r="C174" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
       <c r="D174" t="s">
-        <v>684</v>
+        <v>72</v>
       </c>
       <c r="E174" t="s">
         <v>14</v>
       </c>
       <c r="F174" t="s">
-        <v>698</v>
+        <v>705</v>
       </c>
       <c r="G174" t="s">
-        <v>699</v>
+        <v>706</v>
       </c>
       <c r="H174" t="s">
         <v>406</v>
@@ -8339,24 +8585,27 @@
         <v>407</v>
       </c>
       <c r="J174" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
     </row>
     <row r="175" spans="1:10">
       <c r="A175" t="s">
-        <v>700</v>
+        <v>707</v>
+      </c>
+      <c r="B175" t="s">
+        <v>708</v>
       </c>
       <c r="C175" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
       <c r="D175" t="s">
-        <v>604</v>
+        <v>366</v>
       </c>
       <c r="E175" t="s">
         <v>14</v>
       </c>
       <c r="F175" t="s">
-        <v>701</v>
+        <v>709</v>
       </c>
       <c r="G175" t="s">
         <v>16</v>
@@ -8373,51 +8622,57 @@
     </row>
     <row r="176" spans="1:10">
       <c r="A176" t="s">
-        <v>702</v>
+        <v>710</v>
+      </c>
+      <c r="B176" t="s">
+        <v>711</v>
       </c>
       <c r="C176" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
       <c r="D176" t="s">
-        <v>703</v>
+        <v>712</v>
       </c>
       <c r="E176" t="s">
         <v>14</v>
       </c>
       <c r="F176" t="s">
-        <v>704</v>
+        <v>713</v>
       </c>
       <c r="G176" t="s">
-        <v>705</v>
+        <v>714</v>
       </c>
       <c r="H176" t="s">
         <v>439</v>
       </c>
       <c r="I176" t="s">
-        <v>662</v>
+        <v>666</v>
       </c>
       <c r="J176" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
     </row>
     <row r="177" spans="1:10">
       <c r="A177" t="s">
-        <v>706</v>
+        <v>715</v>
+      </c>
+      <c r="B177" t="s">
+        <v>716</v>
       </c>
       <c r="C177" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
       <c r="D177" t="s">
-        <v>600</v>
+        <v>21</v>
       </c>
       <c r="E177" t="s">
         <v>14</v>
       </c>
       <c r="F177" t="s">
-        <v>707</v>
+        <v>717</v>
       </c>
       <c r="G177" t="s">
-        <v>708</v>
+        <v>718</v>
       </c>
       <c r="H177" t="s">
         <v>439</v>
@@ -8431,19 +8686,22 @@
     </row>
     <row r="178" spans="1:10">
       <c r="A178" t="s">
-        <v>709</v>
+        <v>719</v>
+      </c>
+      <c r="B178" t="s">
+        <v>720</v>
       </c>
       <c r="C178" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
       <c r="D178" t="s">
-        <v>593</v>
+        <v>296</v>
       </c>
       <c r="E178" t="s">
         <v>14</v>
       </c>
       <c r="F178" t="s">
-        <v>583</v>
+        <v>297</v>
       </c>
       <c r="G178" t="s">
         <v>16</v>
@@ -8460,28 +8718,31 @@
     </row>
     <row r="179" spans="1:10">
       <c r="A179" t="s">
-        <v>710</v>
+        <v>721</v>
+      </c>
+      <c r="B179" t="s">
+        <v>722</v>
       </c>
       <c r="C179" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
       <c r="D179" t="s">
-        <v>668</v>
+        <v>64</v>
       </c>
       <c r="E179" t="s">
         <v>14</v>
       </c>
       <c r="F179" t="s">
-        <v>583</v>
+        <v>297</v>
       </c>
       <c r="G179" t="s">
-        <v>584</v>
+        <v>361</v>
       </c>
       <c r="H179" t="s">
-        <v>711</v>
+        <v>723</v>
       </c>
       <c r="I179" t="s">
-        <v>712</v>
+        <v>724</v>
       </c>
       <c r="J179" t="s">
         <v>51</v>
@@ -8489,28 +8750,31 @@
     </row>
     <row r="180" spans="1:10">
       <c r="A180" t="s">
-        <v>713</v>
+        <v>725</v>
+      </c>
+      <c r="B180" t="s">
+        <v>726</v>
       </c>
       <c r="C180" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
       <c r="D180" t="s">
-        <v>622</v>
+        <v>236</v>
       </c>
       <c r="E180" t="s">
         <v>14</v>
       </c>
       <c r="F180" t="s">
-        <v>583</v>
+        <v>297</v>
       </c>
       <c r="G180" t="s">
-        <v>584</v>
+        <v>361</v>
       </c>
       <c r="H180" t="s">
         <v>362</v>
       </c>
       <c r="I180" t="s">
-        <v>714</v>
+        <v>727</v>
       </c>
       <c r="J180" t="s">
         <v>51</v>
@@ -8518,22 +8782,25 @@
     </row>
     <row r="181" spans="1:10">
       <c r="A181" t="s">
-        <v>715</v>
+        <v>728</v>
+      </c>
+      <c r="B181" t="s">
+        <v>729</v>
       </c>
       <c r="C181" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
       <c r="D181" t="s">
-        <v>639</v>
+        <v>170</v>
       </c>
       <c r="E181" t="s">
         <v>14</v>
       </c>
       <c r="F181" t="s">
-        <v>716</v>
+        <v>373</v>
       </c>
       <c r="G181" t="s">
-        <v>717</v>
+        <v>730</v>
       </c>
       <c r="H181" t="s">
         <v>81</v>
@@ -8547,86 +8814,95 @@
     </row>
     <row r="182" spans="1:10">
       <c r="A182" t="s">
-        <v>718</v>
+        <v>731</v>
+      </c>
+      <c r="B182" t="s">
+        <v>732</v>
       </c>
       <c r="C182" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
       <c r="D182" t="s">
-        <v>593</v>
+        <v>296</v>
       </c>
       <c r="E182" t="s">
         <v>14</v>
       </c>
       <c r="F182" t="s">
-        <v>719</v>
+        <v>733</v>
       </c>
       <c r="G182" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="H182" t="s">
         <v>469</v>
       </c>
       <c r="I182" t="s">
-        <v>720</v>
+        <v>734</v>
       </c>
       <c r="J182" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
     </row>
     <row r="183" spans="1:10">
       <c r="A183" t="s">
-        <v>721</v>
+        <v>735</v>
+      </c>
+      <c r="B183" t="s">
+        <v>736</v>
       </c>
       <c r="C183" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
       <c r="D183" t="s">
-        <v>676</v>
+        <v>164</v>
       </c>
       <c r="E183" t="s">
         <v>14</v>
       </c>
       <c r="F183" t="s">
-        <v>722</v>
+        <v>737</v>
       </c>
       <c r="G183" t="s">
-        <v>723</v>
+        <v>738</v>
       </c>
       <c r="H183" t="s">
         <v>81</v>
       </c>
       <c r="I183" t="s">
-        <v>724</v>
+        <v>739</v>
       </c>
       <c r="J183" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
     </row>
     <row r="184" spans="1:10">
       <c r="A184" t="s">
-        <v>725</v>
+        <v>740</v>
+      </c>
+      <c r="B184" t="s">
+        <v>741</v>
       </c>
       <c r="C184" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
       <c r="D184" t="s">
-        <v>588</v>
+        <v>45</v>
       </c>
       <c r="E184" t="s">
         <v>14</v>
       </c>
       <c r="F184" t="s">
-        <v>583</v>
+        <v>297</v>
       </c>
       <c r="G184" t="s">
-        <v>584</v>
+        <v>361</v>
       </c>
       <c r="H184" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="I184" t="s">
-        <v>726</v>
+        <v>742</v>
       </c>
       <c r="J184" t="s">
         <v>51</v>
@@ -8634,19 +8910,22 @@
     </row>
     <row r="185" spans="1:10">
       <c r="A185" t="s">
-        <v>727</v>
+        <v>743</v>
+      </c>
+      <c r="B185" t="s">
+        <v>744</v>
       </c>
       <c r="C185" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
       <c r="D185" t="s">
-        <v>668</v>
+        <v>64</v>
       </c>
       <c r="E185" t="s">
         <v>14</v>
       </c>
       <c r="F185" t="s">
-        <v>728</v>
+        <v>405</v>
       </c>
       <c r="G185" t="s">
         <v>16</v>
@@ -8663,28 +8942,31 @@
     </row>
     <row r="186" spans="1:10">
       <c r="A186" t="s">
-        <v>729</v>
+        <v>745</v>
+      </c>
+      <c r="B186" t="s">
+        <v>746</v>
       </c>
       <c r="C186" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
       <c r="D186" t="s">
-        <v>635</v>
+        <v>55</v>
       </c>
       <c r="E186" t="s">
         <v>14</v>
       </c>
       <c r="F186" t="s">
-        <v>583</v>
+        <v>297</v>
       </c>
       <c r="G186" t="s">
-        <v>584</v>
+        <v>361</v>
       </c>
       <c r="H186" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="I186" t="s">
-        <v>726</v>
+        <v>742</v>
       </c>
       <c r="J186" t="s">
         <v>51</v>
@@ -8692,22 +8974,25 @@
     </row>
     <row r="187" spans="1:10">
       <c r="A187" t="s">
-        <v>730</v>
+        <v>747</v>
+      </c>
+      <c r="B187" t="s">
+        <v>748</v>
       </c>
       <c r="C187" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
       <c r="D187" t="s">
-        <v>631</v>
+        <v>13</v>
       </c>
       <c r="E187" t="s">
         <v>14</v>
       </c>
       <c r="F187" t="s">
-        <v>731</v>
+        <v>749</v>
       </c>
       <c r="G187" t="s">
-        <v>732</v>
+        <v>750</v>
       </c>
       <c r="H187" t="s">
         <v>478</v>
@@ -8721,22 +9006,25 @@
     </row>
     <row r="188" spans="1:10">
       <c r="A188" t="s">
-        <v>733</v>
+        <v>751</v>
+      </c>
+      <c r="B188" t="s">
+        <v>752</v>
       </c>
       <c r="C188" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
       <c r="D188" t="s">
-        <v>613</v>
+        <v>175</v>
       </c>
       <c r="E188" t="s">
         <v>14</v>
       </c>
       <c r="F188" t="s">
-        <v>734</v>
+        <v>460</v>
       </c>
       <c r="G188" t="s">
-        <v>735</v>
+        <v>753</v>
       </c>
       <c r="H188" t="s">
         <v>406</v>
@@ -8750,19 +9038,22 @@
     </row>
     <row r="189" spans="1:10">
       <c r="A189" t="s">
-        <v>736</v>
+        <v>754</v>
+      </c>
+      <c r="B189" t="s">
+        <v>755</v>
       </c>
       <c r="C189" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
       <c r="D189" t="s">
-        <v>588</v>
+        <v>45</v>
       </c>
       <c r="E189" t="s">
         <v>570</v>
       </c>
       <c r="F189" t="s">
-        <v>660</v>
+        <v>664</v>
       </c>
       <c r="G189" t="s">
         <v>16</v>
@@ -8771,7 +9062,7 @@
         <v>439</v>
       </c>
       <c r="I189" t="s">
-        <v>662</v>
+        <v>666</v>
       </c>
       <c r="J189" t="s">
         <v>23</v>
@@ -8779,28 +9070,31 @@
     </row>
     <row r="190" spans="1:10">
       <c r="A190" t="s">
-        <v>737</v>
+        <v>756</v>
+      </c>
+      <c r="B190" t="s">
+        <v>757</v>
       </c>
       <c r="C190" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
       <c r="D190" t="s">
-        <v>609</v>
+        <v>158</v>
       </c>
       <c r="E190" t="s">
         <v>14</v>
       </c>
       <c r="F190" t="s">
-        <v>738</v>
+        <v>758</v>
       </c>
       <c r="G190" t="s">
-        <v>739</v>
+        <v>305</v>
       </c>
       <c r="H190" t="s">
         <v>32</v>
       </c>
       <c r="I190" t="s">
-        <v>740</v>
+        <v>759</v>
       </c>
       <c r="J190" t="s">
         <v>81</v>
@@ -8808,77 +9102,86 @@
     </row>
     <row r="191" spans="1:10">
       <c r="A191" t="s">
-        <v>741</v>
+        <v>760</v>
+      </c>
+      <c r="B191" t="s">
+        <v>761</v>
       </c>
       <c r="C191" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
       <c r="D191" t="s">
-        <v>613</v>
+        <v>175</v>
       </c>
       <c r="E191" t="s">
         <v>570</v>
       </c>
       <c r="F191" t="s">
-        <v>660</v>
+        <v>664</v>
       </c>
       <c r="G191" t="s">
-        <v>742</v>
+        <v>762</v>
       </c>
       <c r="I191" t="s">
-        <v>662</v>
+        <v>666</v>
       </c>
       <c r="J191" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
     </row>
     <row r="192" spans="1:10">
       <c r="A192" t="s">
-        <v>743</v>
+        <v>763</v>
+      </c>
+      <c r="B192" t="s">
+        <v>764</v>
       </c>
       <c r="C192" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
       <c r="D192" t="s">
-        <v>744</v>
+        <v>27</v>
       </c>
       <c r="E192" t="s">
         <v>14</v>
       </c>
       <c r="F192" t="s">
-        <v>614</v>
+        <v>611</v>
       </c>
       <c r="G192" t="s">
-        <v>615</v>
+        <v>612</v>
       </c>
       <c r="H192" t="s">
         <v>81</v>
       </c>
       <c r="I192" t="s">
-        <v>724</v>
+        <v>739</v>
       </c>
       <c r="J192" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
     </row>
     <row r="193" spans="1:10">
       <c r="A193" t="s">
-        <v>745</v>
+        <v>765</v>
+      </c>
+      <c r="B193" t="s">
+        <v>766</v>
       </c>
       <c r="C193" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
       <c r="D193" t="s">
-        <v>600</v>
+        <v>21</v>
       </c>
       <c r="E193" t="s">
         <v>14</v>
       </c>
       <c r="F193" t="s">
-        <v>746</v>
+        <v>388</v>
       </c>
       <c r="G193" t="s">
-        <v>747</v>
+        <v>767</v>
       </c>
       <c r="H193" t="s">
         <v>81</v>
@@ -8892,25 +9195,28 @@
     </row>
     <row r="194" spans="1:10">
       <c r="A194" t="s">
-        <v>748</v>
+        <v>768</v>
+      </c>
+      <c r="B194" t="s">
+        <v>769</v>
       </c>
       <c r="C194" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
       <c r="D194" t="s">
-        <v>582</v>
+        <v>119</v>
       </c>
       <c r="E194" t="s">
         <v>14</v>
       </c>
       <c r="F194" t="s">
-        <v>749</v>
+        <v>770</v>
       </c>
       <c r="G194" t="s">
-        <v>750</v>
+        <v>771</v>
       </c>
       <c r="I194" t="s">
-        <v>616</v>
+        <v>613</v>
       </c>
       <c r="J194" t="s">
         <v>51</v>
@@ -8918,28 +9224,31 @@
     </row>
     <row r="195" spans="1:10">
       <c r="A195" t="s">
-        <v>751</v>
+        <v>772</v>
+      </c>
+      <c r="B195" t="s">
+        <v>773</v>
       </c>
       <c r="C195" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
       <c r="D195" t="s">
-        <v>622</v>
+        <v>236</v>
       </c>
       <c r="E195" t="s">
         <v>14</v>
       </c>
       <c r="F195" t="s">
-        <v>752</v>
+        <v>491</v>
       </c>
       <c r="G195" t="s">
-        <v>753</v>
+        <v>774</v>
       </c>
       <c r="H195" t="s">
-        <v>679</v>
+        <v>682</v>
       </c>
       <c r="I195" t="s">
-        <v>680</v>
+        <v>683</v>
       </c>
       <c r="J195" t="s">
         <v>227</v>
@@ -8947,86 +9256,95 @@
     </row>
     <row r="196" spans="1:10">
       <c r="A196" t="s">
-        <v>754</v>
+        <v>775</v>
+      </c>
+      <c r="B196" t="s">
+        <v>776</v>
       </c>
       <c r="C196" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
       <c r="D196" t="s">
-        <v>582</v>
+        <v>119</v>
       </c>
       <c r="E196" t="s">
         <v>14</v>
       </c>
       <c r="F196" t="s">
-        <v>614</v>
+        <v>611</v>
       </c>
       <c r="G196" t="s">
-        <v>755</v>
+        <v>777</v>
       </c>
       <c r="H196" t="s">
         <v>81</v>
       </c>
       <c r="I196" t="s">
-        <v>724</v>
+        <v>739</v>
       </c>
       <c r="J196" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
     </row>
     <row r="197" spans="1:10">
       <c r="A197" t="s">
-        <v>756</v>
+        <v>778</v>
+      </c>
+      <c r="B197" t="s">
+        <v>779</v>
       </c>
       <c r="C197" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
       <c r="D197" t="s">
-        <v>635</v>
+        <v>55</v>
       </c>
       <c r="E197" t="s">
         <v>14</v>
       </c>
       <c r="F197" t="s">
-        <v>685</v>
+        <v>689</v>
       </c>
       <c r="G197" t="s">
-        <v>757</v>
+        <v>780</v>
       </c>
       <c r="H197" t="s">
+        <v>627</v>
+      </c>
+      <c r="I197" t="s">
         <v>628</v>
       </c>
-      <c r="I197" t="s">
-        <v>629</v>
-      </c>
       <c r="J197" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
     </row>
     <row r="198" spans="1:10">
       <c r="A198" t="s">
-        <v>758</v>
+        <v>781</v>
+      </c>
+      <c r="B198" t="s">
+        <v>782</v>
       </c>
       <c r="C198" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
       <c r="D198" t="s">
-        <v>588</v>
+        <v>45</v>
       </c>
       <c r="E198" t="s">
         <v>14</v>
       </c>
       <c r="F198" t="s">
-        <v>722</v>
+        <v>737</v>
       </c>
       <c r="G198" t="s">
-        <v>759</v>
+        <v>783</v>
       </c>
       <c r="H198" t="s">
         <v>116</v>
       </c>
       <c r="I198" t="s">
-        <v>616</v>
+        <v>613</v>
       </c>
       <c r="J198" t="s">
         <v>227</v>
@@ -9034,28 +9352,31 @@
     </row>
     <row r="199" spans="1:10">
       <c r="A199" t="s">
-        <v>760</v>
+        <v>784</v>
+      </c>
+      <c r="B199" t="s">
+        <v>785</v>
       </c>
       <c r="C199" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
       <c r="D199" t="s">
-        <v>668</v>
+        <v>64</v>
       </c>
       <c r="E199" t="s">
         <v>14</v>
       </c>
       <c r="F199" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="G199" t="s">
-        <v>761</v>
+        <v>786</v>
       </c>
       <c r="H199" t="s">
         <v>161</v>
       </c>
       <c r="I199" t="s">
-        <v>687</v>
+        <v>691</v>
       </c>
       <c r="J199" t="s">
         <v>227</v>
@@ -9063,51 +9384,57 @@
     </row>
     <row r="200" spans="1:10">
       <c r="A200" t="s">
-        <v>762</v>
+        <v>787</v>
+      </c>
+      <c r="B200" t="s">
+        <v>788</v>
       </c>
       <c r="C200" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
       <c r="D200" t="s">
+        <v>45</v>
+      </c>
+      <c r="E200" t="s">
+        <v>14</v>
+      </c>
+      <c r="F200" t="s">
         <v>588</v>
       </c>
-      <c r="E200" t="s">
-        <v>14</v>
-      </c>
-      <c r="F200" t="s">
-        <v>589</v>
-      </c>
       <c r="G200" t="s">
-        <v>708</v>
+        <v>718</v>
       </c>
       <c r="H200" t="s">
         <v>227</v>
       </c>
       <c r="I200" t="s">
-        <v>763</v>
+        <v>789</v>
       </c>
       <c r="J200" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
     </row>
     <row r="201" spans="1:10">
       <c r="A201" t="s">
-        <v>764</v>
+        <v>790</v>
+      </c>
+      <c r="B201" t="s">
+        <v>791</v>
       </c>
       <c r="C201" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
       <c r="D201" t="s">
-        <v>631</v>
+        <v>13</v>
       </c>
       <c r="E201" t="s">
         <v>14</v>
       </c>
       <c r="F201" t="s">
-        <v>731</v>
+        <v>749</v>
       </c>
       <c r="G201" t="s">
-        <v>765</v>
+        <v>792</v>
       </c>
       <c r="H201" t="s">
         <v>406</v>
@@ -9116,30 +9443,33 @@
         <v>407</v>
       </c>
       <c r="J201" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
     </row>
     <row r="202" spans="1:10">
       <c r="A202" t="s">
-        <v>766</v>
+        <v>793</v>
+      </c>
+      <c r="B202" t="s">
+        <v>794</v>
       </c>
       <c r="C202" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
       <c r="D202" t="s">
+        <v>175</v>
+      </c>
+      <c r="E202" t="s">
+        <v>14</v>
+      </c>
+      <c r="F202" t="s">
+        <v>770</v>
+      </c>
+      <c r="G202" t="s">
+        <v>795</v>
+      </c>
+      <c r="I202" t="s">
         <v>613</v>
-      </c>
-      <c r="E202" t="s">
-        <v>14</v>
-      </c>
-      <c r="F202" t="s">
-        <v>749</v>
-      </c>
-      <c r="G202" t="s">
-        <v>767</v>
-      </c>
-      <c r="I202" t="s">
-        <v>616</v>
       </c>
       <c r="J202" t="s">
         <v>51</v>
@@ -9147,22 +9477,25 @@
     </row>
     <row r="203" spans="1:10">
       <c r="A203" t="s">
-        <v>768</v>
+        <v>796</v>
+      </c>
+      <c r="B203" t="s">
+        <v>797</v>
       </c>
       <c r="C203" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
       <c r="D203" t="s">
-        <v>631</v>
+        <v>13</v>
       </c>
       <c r="E203" t="s">
         <v>14</v>
       </c>
       <c r="F203" t="s">
-        <v>673</v>
+        <v>677</v>
       </c>
       <c r="G203" t="s">
-        <v>769</v>
+        <v>798</v>
       </c>
       <c r="H203" t="s">
         <v>406</v>
@@ -9171,27 +9504,30 @@
         <v>407</v>
       </c>
       <c r="J203" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
     </row>
     <row r="204" spans="1:10">
       <c r="A204" t="s">
-        <v>770</v>
+        <v>799</v>
+      </c>
+      <c r="B204" t="s">
+        <v>800</v>
       </c>
       <c r="C204" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
       <c r="D204" t="s">
-        <v>613</v>
+        <v>175</v>
       </c>
       <c r="E204" t="s">
         <v>14</v>
       </c>
       <c r="F204" t="s">
-        <v>771</v>
+        <v>431</v>
       </c>
       <c r="G204" t="s">
-        <v>772</v>
+        <v>801</v>
       </c>
       <c r="H204" t="s">
         <v>81</v>
@@ -9205,54 +9541,60 @@
     </row>
     <row r="205" spans="1:10">
       <c r="A205" t="s">
-        <v>773</v>
+        <v>802</v>
+      </c>
+      <c r="B205" t="s">
+        <v>803</v>
       </c>
       <c r="C205" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
       <c r="D205" t="s">
-        <v>613</v>
+        <v>175</v>
       </c>
       <c r="E205" t="s">
         <v>14</v>
       </c>
       <c r="F205" t="s">
-        <v>722</v>
+        <v>737</v>
       </c>
       <c r="G205" t="s">
-        <v>774</v>
+        <v>804</v>
       </c>
       <c r="H205" t="s">
         <v>81</v>
       </c>
       <c r="I205" t="s">
-        <v>724</v>
+        <v>739</v>
       </c>
       <c r="J205" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
     </row>
     <row r="206" spans="1:10">
       <c r="A206" t="s">
-        <v>775</v>
+        <v>805</v>
+      </c>
+      <c r="B206" t="s">
+        <v>806</v>
       </c>
       <c r="C206" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
       <c r="D206" t="s">
-        <v>618</v>
+        <v>616</v>
       </c>
       <c r="E206" t="s">
         <v>14</v>
       </c>
       <c r="F206" t="s">
-        <v>776</v>
+        <v>807</v>
       </c>
       <c r="G206" t="s">
-        <v>777</v>
+        <v>808</v>
       </c>
       <c r="H206" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="I206" t="s">
         <v>648</v>
@@ -9263,25 +9605,28 @@
     </row>
     <row r="207" spans="1:10">
       <c r="A207" t="s">
-        <v>778</v>
+        <v>809</v>
+      </c>
+      <c r="B207" t="s">
+        <v>810</v>
       </c>
       <c r="C207" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
       <c r="D207" t="s">
-        <v>779</v>
+        <v>811</v>
       </c>
       <c r="E207" t="s">
         <v>14</v>
       </c>
       <c r="F207" t="s">
-        <v>780</v>
+        <v>812</v>
       </c>
       <c r="G207" t="s">
-        <v>781</v>
+        <v>813</v>
       </c>
       <c r="H207" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="I207" t="s">
         <v>648</v>
@@ -9292,28 +9637,31 @@
     </row>
     <row r="208" spans="1:10">
       <c r="A208" t="s">
-        <v>782</v>
+        <v>814</v>
+      </c>
+      <c r="B208" t="s">
+        <v>815</v>
       </c>
       <c r="C208" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
       <c r="D208" t="s">
-        <v>631</v>
+        <v>13</v>
       </c>
       <c r="E208" t="s">
         <v>14</v>
       </c>
       <c r="F208" t="s">
-        <v>722</v>
+        <v>737</v>
       </c>
       <c r="G208" t="s">
-        <v>723</v>
+        <v>738</v>
       </c>
       <c r="H208" t="s">
         <v>116</v>
       </c>
       <c r="I208" t="s">
-        <v>616</v>
+        <v>613</v>
       </c>
       <c r="J208" t="s">
         <v>227</v>
@@ -9321,28 +9669,31 @@
     </row>
     <row r="209" spans="1:10">
       <c r="A209" t="s">
-        <v>783</v>
+        <v>816</v>
+      </c>
+      <c r="B209" t="s">
+        <v>817</v>
       </c>
       <c r="C209" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
       <c r="D209" t="s">
-        <v>784</v>
+        <v>818</v>
       </c>
       <c r="E209" t="s">
         <v>14</v>
       </c>
       <c r="F209" t="s">
-        <v>785</v>
+        <v>819</v>
       </c>
       <c r="G209" t="s">
-        <v>786</v>
+        <v>820</v>
       </c>
       <c r="H209" t="s">
+        <v>595</v>
+      </c>
+      <c r="I209" t="s">
         <v>596</v>
-      </c>
-      <c r="I209" t="s">
-        <v>597</v>
       </c>
       <c r="J209" t="s">
         <v>51</v>
@@ -9350,28 +9701,31 @@
     </row>
     <row r="210" spans="1:10">
       <c r="A210" t="s">
-        <v>787</v>
+        <v>821</v>
+      </c>
+      <c r="B210" t="s">
+        <v>822</v>
       </c>
       <c r="C210" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
       <c r="D210" t="s">
-        <v>631</v>
+        <v>13</v>
       </c>
       <c r="E210" t="s">
         <v>570</v>
       </c>
       <c r="F210" t="s">
-        <v>660</v>
+        <v>664</v>
       </c>
       <c r="G210" t="s">
-        <v>788</v>
+        <v>823</v>
       </c>
       <c r="H210" t="s">
         <v>439</v>
       </c>
       <c r="I210" t="s">
-        <v>662</v>
+        <v>666</v>
       </c>
       <c r="J210" t="s">
         <v>161</v>
@@ -9379,22 +9733,25 @@
     </row>
     <row r="211" spans="1:10">
       <c r="A211" t="s">
-        <v>789</v>
+        <v>824</v>
+      </c>
+      <c r="B211" t="s">
+        <v>825</v>
       </c>
       <c r="C211" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
       <c r="D211" t="s">
-        <v>631</v>
+        <v>13</v>
       </c>
       <c r="E211" t="s">
         <v>14</v>
       </c>
       <c r="F211" t="s">
-        <v>790</v>
+        <v>463</v>
       </c>
       <c r="G211" t="s">
-        <v>791</v>
+        <v>826</v>
       </c>
       <c r="H211" t="s">
         <v>81</v>
@@ -9408,22 +9765,25 @@
     </row>
     <row r="212" spans="1:10">
       <c r="A212" t="s">
-        <v>792</v>
+        <v>827</v>
+      </c>
+      <c r="B212" t="s">
+        <v>828</v>
       </c>
       <c r="C212" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
       <c r="D212" t="s">
-        <v>582</v>
+        <v>119</v>
       </c>
       <c r="E212" t="s">
         <v>14</v>
       </c>
       <c r="F212" t="s">
-        <v>695</v>
+        <v>701</v>
       </c>
       <c r="G212" t="s">
-        <v>793</v>
+        <v>829</v>
       </c>
       <c r="H212" t="s">
         <v>478</v>
@@ -9437,22 +9797,25 @@
     </row>
     <row r="213" spans="1:10">
       <c r="A213" t="s">
-        <v>794</v>
+        <v>830</v>
+      </c>
+      <c r="B213" t="s">
+        <v>831</v>
       </c>
       <c r="C213" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
       <c r="D213" t="s">
-        <v>604</v>
+        <v>366</v>
       </c>
       <c r="E213" t="s">
         <v>14</v>
       </c>
       <c r="F213" t="s">
-        <v>795</v>
+        <v>832</v>
       </c>
       <c r="G213" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="H213" t="s">
         <v>478</v>
@@ -9461,27 +9824,30 @@
         <v>479</v>
       </c>
       <c r="J213" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
     </row>
     <row r="214" spans="1:10">
       <c r="A214" t="s">
-        <v>796</v>
+        <v>833</v>
+      </c>
+      <c r="B214" t="s">
+        <v>834</v>
       </c>
       <c r="C214" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
       <c r="D214" t="s">
-        <v>604</v>
+        <v>366</v>
       </c>
       <c r="E214" t="s">
         <v>14</v>
       </c>
       <c r="F214" t="s">
-        <v>673</v>
+        <v>677</v>
       </c>
       <c r="G214" t="s">
-        <v>797</v>
+        <v>835</v>
       </c>
       <c r="H214" t="s">
         <v>406</v>
@@ -9490,24 +9856,27 @@
         <v>407</v>
       </c>
       <c r="J214" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
     </row>
     <row r="215" spans="1:10">
       <c r="A215" t="s">
-        <v>798</v>
+        <v>836</v>
+      </c>
+      <c r="B215" t="s">
+        <v>837</v>
       </c>
       <c r="C215" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
       <c r="D215" t="s">
-        <v>622</v>
+        <v>236</v>
       </c>
       <c r="E215" t="s">
         <v>14</v>
       </c>
       <c r="F215" t="s">
-        <v>799</v>
+        <v>484</v>
       </c>
       <c r="G215" t="s">
         <v>16</v>
@@ -9524,25 +9893,28 @@
     </row>
     <row r="216" spans="1:10">
       <c r="A216" t="s">
-        <v>800</v>
+        <v>838</v>
+      </c>
+      <c r="B216" t="s">
+        <v>839</v>
       </c>
       <c r="C216" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
       <c r="D216" t="s">
-        <v>588</v>
+        <v>45</v>
       </c>
       <c r="E216" t="s">
         <v>14</v>
       </c>
       <c r="F216" t="s">
-        <v>636</v>
+        <v>840</v>
       </c>
       <c r="G216" t="s">
-        <v>801</v>
+        <v>841</v>
       </c>
       <c r="I216" t="s">
-        <v>616</v>
+        <v>613</v>
       </c>
       <c r="J216" t="s">
         <v>51</v>
@@ -9550,28 +9922,31 @@
     </row>
     <row r="217" spans="1:10">
       <c r="A217" t="s">
-        <v>802</v>
+        <v>842</v>
+      </c>
+      <c r="B217" t="s">
+        <v>843</v>
       </c>
       <c r="C217" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
       <c r="D217" t="s">
-        <v>618</v>
+        <v>616</v>
       </c>
       <c r="E217" t="s">
         <v>14</v>
       </c>
       <c r="F217" t="s">
-        <v>803</v>
+        <v>844</v>
       </c>
       <c r="G217" t="s">
-        <v>804</v>
+        <v>845</v>
       </c>
       <c r="H217" t="s">
-        <v>805</v>
+        <v>846</v>
       </c>
       <c r="I217" t="s">
-        <v>806</v>
+        <v>847</v>
       </c>
       <c r="J217" t="s">
         <v>227</v>
@@ -9579,22 +9954,25 @@
     </row>
     <row r="218" spans="1:10">
       <c r="A218" t="s">
-        <v>807</v>
+        <v>848</v>
+      </c>
+      <c r="B218" t="s">
+        <v>849</v>
       </c>
       <c r="C218" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
       <c r="D218" t="s">
-        <v>600</v>
+        <v>21</v>
       </c>
       <c r="E218" t="s">
         <v>14</v>
       </c>
       <c r="F218" t="s">
-        <v>642</v>
+        <v>473</v>
       </c>
       <c r="G218" t="s">
-        <v>808</v>
+        <v>850</v>
       </c>
       <c r="H218" t="s">
         <v>362</v>
@@ -9608,22 +9986,25 @@
     </row>
     <row r="219" spans="1:10">
       <c r="A219" t="s">
-        <v>809</v>
+        <v>851</v>
+      </c>
+      <c r="B219" t="s">
+        <v>852</v>
       </c>
       <c r="C219" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
       <c r="D219" t="s">
-        <v>609</v>
+        <v>158</v>
       </c>
       <c r="E219" t="s">
         <v>14</v>
       </c>
       <c r="F219" t="s">
-        <v>810</v>
+        <v>559</v>
       </c>
       <c r="G219" t="s">
-        <v>811</v>
+        <v>853</v>
       </c>
       <c r="H219" t="s">
         <v>406</v>
@@ -9637,22 +10018,25 @@
     </row>
     <row r="220" spans="1:10">
       <c r="A220" t="s">
-        <v>812</v>
+        <v>854</v>
+      </c>
+      <c r="B220" t="s">
+        <v>855</v>
       </c>
       <c r="C220" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
       <c r="D220" t="s">
-        <v>609</v>
+        <v>158</v>
       </c>
       <c r="E220" t="s">
         <v>14</v>
       </c>
       <c r="F220" t="s">
-        <v>813</v>
+        <v>856</v>
       </c>
       <c r="G220" t="s">
-        <v>814</v>
+        <v>857</v>
       </c>
       <c r="H220" t="s">
         <v>69</v>
@@ -9661,27 +10045,30 @@
         <v>493</v>
       </c>
       <c r="J220" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
     </row>
     <row r="221" spans="1:10">
       <c r="A221" t="s">
-        <v>815</v>
+        <v>858</v>
+      </c>
+      <c r="B221" t="s">
+        <v>859</v>
       </c>
       <c r="C221" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
       <c r="D221" t="s">
-        <v>744</v>
+        <v>27</v>
       </c>
       <c r="E221" t="s">
         <v>14</v>
       </c>
       <c r="F221" t="s">
-        <v>816</v>
+        <v>514</v>
       </c>
       <c r="G221" t="s">
-        <v>708</v>
+        <v>718</v>
       </c>
       <c r="H221" t="s">
         <v>478</v>
@@ -9695,22 +10082,25 @@
     </row>
     <row r="222" spans="1:10">
       <c r="A222" t="s">
-        <v>817</v>
+        <v>860</v>
+      </c>
+      <c r="B222" t="s">
+        <v>861</v>
       </c>
       <c r="C222" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
       <c r="D222" t="s">
-        <v>639</v>
+        <v>170</v>
       </c>
       <c r="E222" t="s">
         <v>14</v>
       </c>
       <c r="F222" t="s">
-        <v>695</v>
+        <v>701</v>
       </c>
       <c r="G222" t="s">
-        <v>818</v>
+        <v>862</v>
       </c>
       <c r="H222" t="s">
         <v>406</v>
@@ -9719,33 +10109,36 @@
         <v>407</v>
       </c>
       <c r="J222" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
     </row>
     <row r="223" spans="1:10">
       <c r="A223" t="s">
-        <v>819</v>
+        <v>863</v>
+      </c>
+      <c r="B223" t="s">
+        <v>864</v>
       </c>
       <c r="C223" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
       <c r="D223" t="s">
-        <v>604</v>
+        <v>366</v>
       </c>
       <c r="E223" t="s">
         <v>14</v>
       </c>
       <c r="F223" t="s">
-        <v>813</v>
+        <v>856</v>
       </c>
       <c r="G223" t="s">
-        <v>820</v>
+        <v>865</v>
       </c>
       <c r="H223" t="s">
-        <v>679</v>
+        <v>682</v>
       </c>
       <c r="I223" t="s">
-        <v>680</v>
+        <v>683</v>
       </c>
       <c r="J223" t="s">
         <v>227</v>
@@ -9753,28 +10146,31 @@
     </row>
     <row r="224" spans="1:10">
       <c r="A224" t="s">
-        <v>821</v>
+        <v>866</v>
+      </c>
+      <c r="B224" t="s">
+        <v>867</v>
       </c>
       <c r="C224" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
       <c r="D224" t="s">
-        <v>593</v>
+        <v>296</v>
       </c>
       <c r="E224" t="s">
         <v>14</v>
       </c>
       <c r="F224" t="s">
-        <v>583</v>
+        <v>297</v>
       </c>
       <c r="G224" t="s">
-        <v>822</v>
+        <v>868</v>
       </c>
       <c r="H224" t="s">
         <v>91</v>
       </c>
       <c r="I224" t="s">
-        <v>823</v>
+        <v>869</v>
       </c>
       <c r="J224" t="s">
         <v>227</v>
@@ -9782,22 +10178,25 @@
     </row>
     <row r="225" spans="1:10">
       <c r="A225" t="s">
-        <v>824</v>
+        <v>870</v>
+      </c>
+      <c r="B225" t="s">
+        <v>871</v>
       </c>
       <c r="C225" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
       <c r="D225" t="s">
-        <v>609</v>
+        <v>158</v>
       </c>
       <c r="E225" t="s">
         <v>14</v>
       </c>
       <c r="F225" t="s">
-        <v>623</v>
+        <v>621</v>
       </c>
       <c r="G225" t="s">
-        <v>825</v>
+        <v>872</v>
       </c>
       <c r="H225" t="s">
         <v>406</v>
@@ -9806,33 +10205,36 @@
         <v>407</v>
       </c>
       <c r="J225" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
     </row>
     <row r="226" spans="1:10">
       <c r="A226" t="s">
-        <v>826</v>
+        <v>873</v>
+      </c>
+      <c r="B226" t="s">
+        <v>874</v>
       </c>
       <c r="C226" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
       <c r="D226" t="s">
-        <v>631</v>
+        <v>13</v>
       </c>
       <c r="E226" t="s">
         <v>14</v>
       </c>
       <c r="F226" t="s">
-        <v>614</v>
+        <v>611</v>
       </c>
       <c r="G226" t="s">
-        <v>827</v>
+        <v>875</v>
       </c>
       <c r="H226" t="s">
         <v>116</v>
       </c>
       <c r="I226" t="s">
-        <v>616</v>
+        <v>613</v>
       </c>
       <c r="J226" t="s">
         <v>227</v>
@@ -9840,28 +10242,31 @@
     </row>
     <row r="227" spans="1:10">
       <c r="A227" t="s">
-        <v>828</v>
+        <v>876</v>
+      </c>
+      <c r="B227" t="s">
+        <v>877</v>
       </c>
       <c r="C227" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
       <c r="D227" t="s">
-        <v>618</v>
+        <v>616</v>
       </c>
       <c r="E227" t="s">
         <v>14</v>
       </c>
       <c r="F227" t="s">
-        <v>829</v>
+        <v>878</v>
       </c>
       <c r="G227" t="s">
-        <v>830</v>
+        <v>879</v>
       </c>
       <c r="H227" t="s">
+        <v>595</v>
+      </c>
+      <c r="I227" t="s">
         <v>596</v>
-      </c>
-      <c r="I227" t="s">
-        <v>597</v>
       </c>
       <c r="J227" t="s">
         <v>51</v>
@@ -9869,22 +10274,25 @@
     </row>
     <row r="228" spans="1:10">
       <c r="A228" t="s">
-        <v>831</v>
+        <v>880</v>
+      </c>
+      <c r="B228" t="s">
+        <v>881</v>
       </c>
       <c r="C228" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
       <c r="D228" t="s">
-        <v>613</v>
+        <v>175</v>
       </c>
       <c r="E228" t="s">
         <v>14</v>
       </c>
       <c r="F228" t="s">
-        <v>698</v>
+        <v>705</v>
       </c>
       <c r="G228" t="s">
-        <v>832</v>
+        <v>882</v>
       </c>
       <c r="H228" t="s">
         <v>478</v>
@@ -9898,28 +10306,31 @@
     </row>
     <row r="229" spans="1:10">
       <c r="A229" t="s">
-        <v>833</v>
+        <v>883</v>
+      </c>
+      <c r="B229" t="s">
+        <v>884</v>
       </c>
       <c r="C229" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
       <c r="D229" t="s">
-        <v>834</v>
+        <v>885</v>
       </c>
       <c r="E229" t="s">
         <v>14</v>
       </c>
       <c r="F229" t="s">
-        <v>835</v>
+        <v>886</v>
       </c>
       <c r="G229" t="s">
         <v>16</v>
       </c>
       <c r="H229" t="s">
+        <v>595</v>
+      </c>
+      <c r="I229" t="s">
         <v>596</v>
-      </c>
-      <c r="I229" t="s">
-        <v>597</v>
       </c>
       <c r="J229" t="s">
         <v>23</v>
@@ -9927,28 +10338,31 @@
     </row>
     <row r="230" spans="1:10">
       <c r="A230" t="s">
-        <v>836</v>
+        <v>887</v>
+      </c>
+      <c r="B230" t="s">
+        <v>888</v>
       </c>
       <c r="C230" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
       <c r="D230" t="s">
-        <v>837</v>
+        <v>889</v>
       </c>
       <c r="E230" t="s">
         <v>570</v>
       </c>
       <c r="F230" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="G230" t="s">
         <v>16</v>
       </c>
       <c r="H230" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="I230" t="s">
-        <v>620</v>
+        <v>618</v>
       </c>
       <c r="J230" t="s">
         <v>23</v>
@@ -9956,28 +10370,31 @@
     </row>
     <row r="231" spans="1:10">
       <c r="A231" t="s">
-        <v>838</v>
+        <v>890</v>
+      </c>
+      <c r="B231" t="s">
+        <v>891</v>
       </c>
       <c r="C231" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
       <c r="D231" t="s">
-        <v>837</v>
+        <v>889</v>
       </c>
       <c r="E231" t="s">
         <v>570</v>
       </c>
       <c r="F231" t="s">
-        <v>839</v>
+        <v>892</v>
       </c>
       <c r="G231" t="s">
         <v>16</v>
       </c>
       <c r="H231" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="I231" t="s">
-        <v>620</v>
+        <v>618</v>
       </c>
       <c r="J231" t="s">
         <v>23</v>

</xml_diff>

<commit_message>
Show key quests by rating. Edit typo.
</commit_message>
<xml_diff>
--- a/data_G.xlsx
+++ b/data_G.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2282" uniqueCount="893">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2310" uniqueCount="893">
   <si>
     <t>questName</t>
   </si>
@@ -76,6 +76,9 @@
     <t>3600z</t>
   </si>
   <si>
+    <t>0z</t>
+  </si>
+  <si>
     <t>原生林の採集ツアー</t>
   </si>
   <si>
@@ -86,9 +89,6 @@
   </si>
   <si>
     <t>타임업 혹은 고양이택시티켓(ネコタクチケット) 납품</t>
-  </si>
-  <si>
-    <t>0z</t>
   </si>
   <si>
     <t>12z</t>
@@ -3074,8 +3074,8 @@
   <dimension ref="A1:J231"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
-      <pane ySplit="1" topLeftCell="B200" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G206" sqref="G206"/>
+      <pane ySplit="1" topLeftCell="F159" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H164" sqref="H164"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3152,34 +3152,40 @@
       <c r="I2" t="s">
         <v>18</v>
       </c>
+      <c r="J2" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="3" spans="1:10">
       <c r="A3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C3" t="s">
         <v>12</v>
       </c>
       <c r="D3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E3" t="s">
         <v>14</v>
       </c>
       <c r="F3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G3" t="s">
         <v>16</v>
       </c>
       <c r="H3" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="I3" t="s">
         <v>24</v>
+      </c>
+      <c r="J3" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -3242,6 +3248,9 @@
       <c r="I5" t="s">
         <v>37</v>
       </c>
+      <c r="J5" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" t="s">
@@ -3260,16 +3269,19 @@
         <v>14</v>
       </c>
       <c r="F6" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G6" t="s">
         <v>16</v>
       </c>
       <c r="H6" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="I6" t="s">
         <v>24</v>
+      </c>
+      <c r="J6" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -3289,16 +3301,19 @@
         <v>14</v>
       </c>
       <c r="F7" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G7" t="s">
         <v>16</v>
       </c>
       <c r="H7" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="I7" t="s">
         <v>24</v>
+      </c>
+      <c r="J7" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -3318,16 +3333,19 @@
         <v>14</v>
       </c>
       <c r="F8" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G8" t="s">
         <v>16</v>
       </c>
       <c r="H8" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="I8" t="s">
         <v>24</v>
+      </c>
+      <c r="J8" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -3411,16 +3429,19 @@
         <v>14</v>
       </c>
       <c r="F11" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G11" t="s">
         <v>16</v>
       </c>
       <c r="H11" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="I11" t="s">
         <v>24</v>
+      </c>
+      <c r="J11" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:10">
@@ -3594,7 +3615,7 @@
         <v>12</v>
       </c>
       <c r="D17" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E17" t="s">
         <v>14</v>
@@ -3696,16 +3717,19 @@
         <v>14</v>
       </c>
       <c r="F20" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G20" t="s">
         <v>16</v>
       </c>
       <c r="H20" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="I20" t="s">
         <v>24</v>
+      </c>
+      <c r="J20" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="21" spans="1:10">
@@ -3768,6 +3792,9 @@
       <c r="I22" t="s">
         <v>116</v>
       </c>
+      <c r="J22" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="23" spans="1:10">
       <c r="A23" t="s">
@@ -3786,16 +3813,19 @@
         <v>14</v>
       </c>
       <c r="F23" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G23" t="s">
         <v>16</v>
       </c>
       <c r="H23" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="I23" t="s">
         <v>24</v>
+      </c>
+      <c r="J23" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="24" spans="1:10">
@@ -3911,16 +3941,19 @@
         <v>14</v>
       </c>
       <c r="F27" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G27" t="s">
         <v>16</v>
       </c>
       <c r="H27" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="I27" t="s">
         <v>24</v>
+      </c>
+      <c r="J27" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="28" spans="1:10">
@@ -3940,16 +3973,19 @@
         <v>14</v>
       </c>
       <c r="F28" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G28" t="s">
         <v>16</v>
       </c>
       <c r="H28" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="I28" t="s">
         <v>24</v>
+      </c>
+      <c r="J28" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="29" spans="1:10">
@@ -4353,16 +4389,19 @@
         <v>14</v>
       </c>
       <c r="F41" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G41" t="s">
         <v>16</v>
       </c>
       <c r="H41" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="I41" t="s">
         <v>24</v>
+      </c>
+      <c r="J41" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="42" spans="1:10">
@@ -4617,6 +4656,9 @@
       <c r="I49" t="s">
         <v>32</v>
       </c>
+      <c r="J49" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="50" spans="1:10">
       <c r="A50" t="s">
@@ -4646,6 +4688,9 @@
       <c r="I50" t="s">
         <v>227</v>
       </c>
+      <c r="J50" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="51" spans="1:10">
       <c r="A51" t="s">
@@ -4760,16 +4805,19 @@
         <v>14</v>
       </c>
       <c r="F54" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G54" t="s">
         <v>16</v>
       </c>
       <c r="H54" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="I54" t="s">
         <v>24</v>
+      </c>
+      <c r="J54" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="55" spans="1:10">
@@ -4789,16 +4837,19 @@
         <v>14</v>
       </c>
       <c r="F55" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G55" t="s">
         <v>16</v>
       </c>
       <c r="H55" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="I55" t="s">
         <v>24</v>
+      </c>
+      <c r="J55" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="56" spans="1:10">
@@ -4829,6 +4880,9 @@
       <c r="I56" t="s">
         <v>246</v>
       </c>
+      <c r="J56" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="57" spans="1:10">
       <c r="A57" t="s">
@@ -4905,7 +4959,7 @@
         <v>157</v>
       </c>
       <c r="D59" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E59" t="s">
         <v>14</v>
@@ -5129,7 +5183,7 @@
         <v>157</v>
       </c>
       <c r="D66" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E66" t="s">
         <v>14</v>
@@ -5231,16 +5285,19 @@
         <v>14</v>
       </c>
       <c r="F69" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G69" t="s">
         <v>16</v>
       </c>
       <c r="H69" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="I69" t="s">
         <v>24</v>
+      </c>
+      <c r="J69" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="70" spans="1:10">
@@ -5452,16 +5509,19 @@
         <v>14</v>
       </c>
       <c r="F76" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G76" t="s">
         <v>16</v>
       </c>
       <c r="H76" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="I76" t="s">
         <v>24</v>
+      </c>
+      <c r="J76" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="77" spans="1:10">
@@ -5635,7 +5695,7 @@
         <v>157</v>
       </c>
       <c r="D82" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E82" t="s">
         <v>14</v>
@@ -5651,6 +5711,9 @@
       </c>
       <c r="I82" t="s">
         <v>18</v>
+      </c>
+      <c r="J82" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="83" spans="1:10">
@@ -5932,13 +5995,13 @@
         <v>385</v>
       </c>
       <c r="H91" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="I91" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="J91" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="92" spans="1:10">
@@ -6130,7 +6193,7 @@
         <v>398</v>
       </c>
       <c r="J97" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="98" spans="1:10">
@@ -6240,7 +6303,7 @@
         <v>360</v>
       </c>
       <c r="D101" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E101" t="s">
         <v>14</v>
@@ -6258,7 +6321,7 @@
         <v>424</v>
       </c>
       <c r="J101" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="102" spans="1:10">
@@ -6272,7 +6335,7 @@
         <v>360</v>
       </c>
       <c r="D102" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E102" t="s">
         <v>14</v>
@@ -6482,7 +6545,7 @@
         <v>398</v>
       </c>
       <c r="J108" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="109" spans="1:10">
@@ -6514,7 +6577,7 @@
         <v>454</v>
       </c>
       <c r="J109" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="110" spans="1:10">
@@ -6624,7 +6687,7 @@
         <v>360</v>
       </c>
       <c r="D113" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E113" t="s">
         <v>14</v>
@@ -6738,7 +6801,7 @@
         <v>369</v>
       </c>
       <c r="J116" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="117" spans="1:10">
@@ -6912,7 +6975,7 @@
         <v>360</v>
       </c>
       <c r="D122" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E122" t="s">
         <v>14</v>
@@ -6994,7 +7057,7 @@
         <v>146</v>
       </c>
       <c r="J124" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="125" spans="1:10">
@@ -7046,16 +7109,19 @@
         <v>14</v>
       </c>
       <c r="F126" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G126" t="s">
         <v>16</v>
       </c>
       <c r="H126" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="I126" t="s">
         <v>24</v>
+      </c>
+      <c r="J126" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="127" spans="1:10">
@@ -7197,7 +7263,7 @@
         <v>360</v>
       </c>
       <c r="D131" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E131" t="s">
         <v>14</v>
@@ -7599,7 +7665,7 @@
         <v>572</v>
       </c>
       <c r="J143" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="144" spans="1:10">
@@ -7727,7 +7793,7 @@
         <v>590</v>
       </c>
       <c r="J147" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="148" spans="1:10">
@@ -7773,7 +7839,7 @@
         <v>582</v>
       </c>
       <c r="D149" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E149" t="s">
         <v>14</v>
@@ -7919,7 +7985,7 @@
         <v>618</v>
       </c>
       <c r="J153" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="154" spans="1:10">
@@ -8079,7 +8145,7 @@
         <v>369</v>
       </c>
       <c r="J158" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="159" spans="1:10">
@@ -8157,7 +8223,7 @@
         <v>582</v>
       </c>
       <c r="D161" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E161" t="s">
         <v>14</v>
@@ -8207,7 +8273,7 @@
         <v>657</v>
       </c>
       <c r="J162" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="163" spans="1:10">
@@ -8264,6 +8330,9 @@
       <c r="G164" t="s">
         <v>665</v>
       </c>
+      <c r="H164" t="s">
+        <v>19</v>
+      </c>
       <c r="I164" t="s">
         <v>666</v>
       </c>
@@ -8421,6 +8490,9 @@
       <c r="G169" t="s">
         <v>686</v>
       </c>
+      <c r="H169" t="s">
+        <v>19</v>
+      </c>
       <c r="I169" t="s">
         <v>613</v>
       </c>
@@ -8535,7 +8607,7 @@
         <v>582</v>
       </c>
       <c r="D173" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E173" t="s">
         <v>14</v>
@@ -8617,7 +8689,7 @@
         <v>263</v>
       </c>
       <c r="J175" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="176" spans="1:10">
@@ -8663,7 +8735,7 @@
         <v>582</v>
       </c>
       <c r="D177" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E177" t="s">
         <v>14</v>
@@ -8713,7 +8785,7 @@
         <v>444</v>
       </c>
       <c r="J178" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="179" spans="1:10">
@@ -8937,7 +9009,7 @@
         <v>58</v>
       </c>
       <c r="J185" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="186" spans="1:10">
@@ -9065,7 +9137,7 @@
         <v>666</v>
       </c>
       <c r="J189" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="190" spans="1:10">
@@ -9122,6 +9194,9 @@
       <c r="G191" t="s">
         <v>762</v>
       </c>
+      <c r="H191" t="s">
+        <v>19</v>
+      </c>
       <c r="I191" t="s">
         <v>666</v>
       </c>
@@ -9172,7 +9247,7 @@
         <v>582</v>
       </c>
       <c r="D193" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E193" t="s">
         <v>14</v>
@@ -9215,6 +9290,9 @@
       <c r="G194" t="s">
         <v>771</v>
       </c>
+      <c r="H194" t="s">
+        <v>19</v>
+      </c>
       <c r="I194" t="s">
         <v>613</v>
       </c>
@@ -9468,6 +9546,9 @@
       <c r="G202" t="s">
         <v>795</v>
       </c>
+      <c r="H202" t="s">
+        <v>19</v>
+      </c>
       <c r="I202" t="s">
         <v>613</v>
       </c>
@@ -9888,7 +9969,7 @@
         <v>263</v>
       </c>
       <c r="J215" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="216" spans="1:10">
@@ -9913,6 +9994,9 @@
       <c r="G216" t="s">
         <v>841</v>
       </c>
+      <c r="H216" t="s">
+        <v>19</v>
+      </c>
       <c r="I216" t="s">
         <v>613</v>
       </c>
@@ -9963,7 +10047,7 @@
         <v>582</v>
       </c>
       <c r="D218" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E218" t="s">
         <v>14</v>
@@ -10333,7 +10417,7 @@
         <v>596</v>
       </c>
       <c r="J229" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="230" spans="1:10">
@@ -10365,7 +10449,7 @@
         <v>618</v>
       </c>
       <c r="J230" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="231" spans="1:10">
@@ -10397,7 +10481,7 @@
         <v>618</v>
       </c>
       <c r="J231" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Completed translation of Kariwaza information. Edit typo.
</commit_message>
<xml_diff>
--- a/data_G.xlsx
+++ b/data_G.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19007"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19017"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
@@ -2098,7 +2098,7 @@
     <t>騎士と氷海の決闘</t>
   </si>
   <si>
-    <t>기사와 빙해와 결전</t>
+    <t>기사와 빙해의 결전</t>
   </si>
   <si>
     <t>베리오로스(ベリオロス)의 머리와 가시 파괴</t>
@@ -3074,8 +3074,8 @@
   <dimension ref="A1:J231"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
-      <pane ySplit="1" topLeftCell="F159" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H164" sqref="H164"/>
+      <pane ySplit="1" topLeftCell="A158" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B172" sqref="B172"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>